<commit_message>
Refactor music lyrics generation template; enhance clarity and pedagogical structure
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'Introduction': "Learn to say your name, it's easy and clear, In English, let's start, have no fear.", 'Refrain': "Hello, my name is (Bonjour, je m'appelle), Nice to meet you (Enchanté), let's begin!", 'Dialogue': "Personnage A: What's your name? (Quel est ton nom?)\nPersonnage B: My name is John (Je m'appelle John), nice to meet you (enchanté).\nPersonnage A: I'm Lisa (Je suis Lisa), how are you? (Comment ça va?)\nPersonnage B: I'm good, thank you (Je vais bien, merci)."}</t>
+          <t>{'Introduction': "Hello! My name is... (Bonjour ! Je m'appelle...)", 'Refrain': "What's your name? Nice to meet you! (Quel est ton nom ? Enchanté de te rencontrer !)", 'Couplet': "Personnage A: Hi! I'm Anna. (Salut ! Je m'appelle Anna.)\nPersonnage B: Nice to meet you, Anna. I'm Tom. (Enchanté de te rencontrer, Anna. Je m'appelle Tom.)\nPersonnage A: What's your name? (Quel est ton nom ?)\nPersonnage B: My name is Tom. (Je m'appelle Tom.)\nPersonnage A: Pleased to meet you, Tom. (Ravi de te rencontrer, Tom.)\nPersonnage B: Let's start a conversation. (Commençons une conversation.)"}</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to say your age, it's easy and fun! (Apprenons à dire ton âge, c'est facile et amusant!)", 'Refrain': "I am ... years old, that's how you say it bold! (J'ai ... ans, c'est comme ça qu'on le dit fort!)", 'Dialogue': "Personnage A: How old are you? (Quel âge as-tu?)\nPersonnage B: I am 10 years old. (J'ai 10 ans.)\nPersonnage A: How old is your brother? (Quel âge a ton frère?)\nPersonnage B: He is 15 years old. (Il a 15 ans.)"}</t>
+          <t>{'Introduction': "Yo, listen up, it's time to engage, We're learning how to say our age!", 'Refrain': "I am five years old (J'ai cinq ans), I am ten years old (J'ai dix ans), Use 'I am' and numbers (Utilise 'I am' et les chiffres), that's how it's told (c'est comme ça qu'on le dit).", 'Dialogue': "Personnage A: Hey, how old are you? (Hé, quel âge as-tu ?) Personnage B: I am seven years old (J'ai sept ans), how about you? (et toi ?) Personnage A: I am eight years old (J'ai huit ans), that's cool, right? (c'est cool, non ?) Personnage B: Yeah, my sister is nine (Oui, ma sœur a neuf ans), she's out of sight! (elle est géniale !) Personnage A: My brother is ten (Mon frère a dix ans), he's really tall (il est vraiment grand). Personnage B: Wow, that's great! (Waouh, c'est super !) Let's learn them all! (Apprenons-les tous !)"}</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>{'Introduction': "Apprends à dire ta nationalité, c'est facile, suis-moi !", 'Refrain': 'I am French (Je suis Français), I am Spanish (Je suis Espagnol), I am Italian (Je suis Italien), I am German (Je suis Allemand), I am American (Je suis Américain).', 'Couplet': "Personnage A: What's your nationality? (Quelle est ta nationalité?)\nPersonnage B: I am French (Je suis Français).\nPersonnage A: And you? (Et toi?)\nPersonnage B: I am Spanish (Je suis Espagnol).\nPersonnage A: Nice to meet you! (Enchanté!)"}</t>
+          <t>{'Introduction': "Yo, let's learn how to say your nationality, (Yo, apprenons à dire ta nationalité,) in English, it's easy, you'll see! (en anglais, c'est facile, tu verras!)", 'Refrain': "I am [nationality], that's the way to say, (Je suis [nationalité], c'est comme ça qu'on dit,) 'I am French', 'I am American', every day! (Je suis Français, Je suis Américain, chaque jour!)", 'Couplet': "Personnage A: Hey, what's your name? (Hé, comment tu t'appelles?)\nPersonnage B: My name is Anna, and I am Italian. (Je m'appelle Anna, et je suis Italienne.)\nPersonnage A: Cool! I am John, and I am Canadian. (Cool! Je m'appelle John, et je suis Canadien.)\nPersonnage B: Nice to meet you, John! (Enchantée de te rencontrer, John!)\nPersonnage A: Likewise, Anna! (Moi de même, Anna!)", 'Outro': "With practice, you'll express your nationality, (Avec de la pratique, tu exprimeras ta nationalité,) simply and clearly, that's the key! (simplement et clairement, c'est la clé!)"}</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>{'Introduction': "Apprenons à poser des questions, c'est la clé pour communiquer.", 'Refrain': "What's your name? (Comment tu t'appelles ?) How old are you? (Quel âge as-tu ?)", 'Couplet': "Personnage A: Hi, what's your name? (Salut, comment tu t'appelles ?) Personnage B: My name is Anna. (Je m'appelle Anna.) Personnage A: How old are you, Anna? (Quel âge as-tu, Anna ?) Personnage B: I'm ten years old. (J'ai dix ans.)"}</t>
+          <t>{'Introduction': "Yo, apprendre à poser des questions, c'est essentiel (important).", 'Refrain': "Répète et pratique, pour t'améliorer chaque jour (every day).", 'Couplet': "Personnage A: Hey, what's your name? (Comment tu t'appelles ?)\nPersonnage B: My name is Anna (Je m'appelle Anna).\nPersonnage A: Nice to meet you, Anna (Enchanté, Anna).\nPersonnage A: How old are you? (Quel âge as-tu ?)\nPersonnage B: I'm ten years old (J'ai dix ans).\nPersonnage A: Cool, let's play! (Super, jouons !)\nPersonnage A: What's your favorite color? (Quelle est ta couleur préférée ?)\nPersonnage B: Blue, like the sky (Bleu, comme le ciel).\nPersonnage A: Great choice! (Bon choix !)", 'Conclusion': "Avec la pratique, tu seras à l'aise pour poser ces questions (questions)."}</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to say where you live in English.", 'Refrain': "I live in a place, it's easy to say. (J'habite à un endroit, c'est facile à dire.)", 'Dialogue': "Personnage A: Where do you live? (Où habites-tu?)\nPersonnage B: I live in Paris. (J'habite à Paris.)\nPersonnage A: Do you live in a city? (Habites-tu dans une ville?)\nPersonnage B: Yes, I live in a city. (Oui, j'habite dans une ville.)\nPersonnage A: Is it big or small? (Est-ce grand ou petit?)\nPersonnage B: It's big, like New York. (C'est grand, comme New York.)"}</t>
+          <t>{'Introduction': "Yo, let's learn how to say where you live, it's a basic skill, let's give it a spin!", 'Refrain': "I live in Paris (J'habite à Paris), I live in France (J'habite en France), I live in New York (J'habite à New York), I live in the United States (J'habite aux États-Unis).", 'Dialogue': "Personnage A: Hey, where do you live? (Hé, où habites-tu?)\nPersonnage B: I live in London. (J'habite à Londres.)\nPersonnage A: Oh cool, I live in a small town. (Oh cool, j'habite dans une petite ville.)\nPersonnage B: Do you like it there? (Aimes-tu là-bas?)\nPersonnage A: Yes, it's nice. I live in the countryside. (Oui, c'est sympa. J'habite à la campagne.)\nPersonnage B: I live in the capital city. (J'habite dans la capitale.)\nPersonnage A: That's exciting! (C'est excitant!)"}</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>{'Introduction': "Learn to say goodbye, it's easy and fun!", 'Refrain': 'Goodbye, bye, see you soon (Au revoir, à bientôt), Take care, have a nice day (Prends soin de toi, bonne journée).', 'Couplet': "Personnage A: Hi, I'm leaving now (Salut, je pars maintenant). Personnage B: Goodbye, see you later (Au revoir, à plus tard). Personnage A: Bye, have a nice day (Salut, passe une bonne journée). Personnage B: Take care, see you soon (Prends soin de toi, à bientôt)."}</t>
+          <t>{'Introduction': "Let's learn to say goodbye (au revoir) in English, it's easy and fun!", 'Refrain': 'Goodbye, see you soon (À bientôt), Take care, have a nice afternoon (Bonne après-midi).', 'Dialogue': "Personnage A: Hey, it's time to go. Goodbye! (Hé, il est temps de partir. Au revoir!)\nPersonnage B: Goodbye! See you tomorrow! (Au revoir! À demain!)\nPersonnage A: I'm leaving now. Take care! (Je pars maintenant. Prends soin de toi!)\nPersonnage B: You too, have a nice day! (Toi aussi, passe une bonne journée!)\nPersonnage A: Bye, catch you later! (Salut, à plus tard!)\nPersonnage B: Later! Have a good one! (À plus! Bonne journée!)"}</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn polite words, it's fun and cool! (Apprenons des mots polis, c'est amusant et cool!)", 'Refrain': "Thank you, please, magic words to use, (Merci, s'il vous plaît, des mots magiques à utiliser,) Be polite, it's the way to choose. (Sois poli, c'est la voie à choisir.)", 'Couplet sous forme de dialogue': "Personnage A: Can you help me, please? (Peux-tu m'aider, s'il te plaît?) Personnage B: Sure, thank you for asking! (Bien sûr, merci de demander!) Personnage A: You're welcome, anytime! (De rien, n'importe quand!)"}</t>
+          <t>{'Introduction': "Yo, apprenons les mots de politesse, c'est essentiel pour l'anglais, pas de stress.", 'Refrain': 'La politesse est la clé, dans chaque interaction, en anglais comme ailleurs.', 'Dialogue': "Personnage A: Hey, could you pass the salt, please? (Hé, pourrais-tu passer le sel, s'il te plaît?)\nPersonnage B: Sure, here you go. Thank you for asking! (Bien sûr, voilà. Merci d'avoir demandé!)\nPersonnage A: You're welcome! (De rien!)\nPersonnage B: Excuse me, do you have the time? (Excusez-moi, avez-vous l'heure?)\nPersonnage A: Sorry, I don't have a watch. (Désolé, je n'ai pas de montre.)\nPersonnage B: No problem, thanks anyway! (Pas de problème, merci quand même!)\nPersonnage A: May I sit here? (Puis-je m'asseoir ici?)\nPersonnage B: Yes, please do. (Oui, je vous en prie.)", 'Conclusion': 'Pratiquez ces expressions, et la politesse sera votre alliée.'}</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, let's learn how to say 'How are you?' (Yo, apprenons à dire 'Comment ça va ?')", 'Refrain': "I'm good, I'm okay, I'm not so good (Ça va bien, pas mal, ça va mal)", 'Couplet sous forme de dialogue': "Personnage A: Hey, how are you? (Hé, comment ça va ?)\nPersonnage B: I'm good, thanks! (Ça va bien, merci !)\nPersonnage A: How are you today? (Comment ça va aujourd'hui ?)\nPersonnage B: I'm okay, just tired. (Pas mal, juste fatigué.)\nPersonnage A: How's it going? (Comment ça va ?)\nPersonnage B: I'm not so good, feeling sick. (Ça va mal, je me sens malade.)", 'Refrain (répété à l’identique)': "I'm good, I'm okay, I'm not so good (Ça va bien, pas mal, ça va mal)"}</t>
+          <t>{'Introduction': "Yo, apprenons à répondre à 'Comment ça va ?' en anglais, c'est essentiel (Yo, apprenons à répondre à 'Comment ça va ?' en anglais, c'est essentiel).", 'Refrain': "Exprime tes sentiments, avec le bon ton, c'est important (Exprime tes sentiments, avec le bon ton, c'est important).", 'Couplet 1': "Personnage A: Hey, how are you? (Hey, comment ça va ?)\nPersonnage B: I'm good, thanks! (Ça va bien, merci !)\nPersonnage A: How's your day? (Comment se passe ta journée ?)\nPersonnage B: I'm fine, just working. (Ça va, je travaille juste.)\nPersonnage A: Feeling well today? (Tu te sens bien aujourd'hui ?)\nPersonnage B: Yes, I'm well, and you? (Oui, je vais bien, et toi ?)", 'Couplet 2': "Personnage A: How are things? (Comment ça va ?)\nPersonnage B: Not bad, just a bit tired. (Pas mal, juste un peu fatigué.)\nPersonnage A: Are you okay? (Ça va ?)\nPersonnage B: I'm okay, just busy. (Ça va, juste occupé.)\nPersonnage A: Everything alright? (Tout va bien ?)\nPersonnage B: I'm alright, thanks for asking. (Ça va, merci de demander.)", 'Couplet 3': "Personnage A: How are you feeling? (Comment te sens-tu ?)\nPersonnage B: I'm not so good, a bit sick. (Je ne vais pas très bien, un peu malade.)\nPersonnage A: Anything wrong? (Quelque chose ne va pas ?)\nPersonnage B: I'm not great, had a rough day. (Je ne vais pas bien, j'ai eu une journée difficile.)\nPersonnage A: Need any help? (Besoin d'aide ?)\nPersonnage B: I'm not well, but I'll manage. (Je ne vais pas bien, mais je vais gérer.)", 'Conclusion': 'Ces phrases simples te guideront dans chaque conversation (Ces phrases simples te guideront dans chaque conversation).'}</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn how to greet, in English, it's neat!", 'Refrain': "Good morning (Bonjour), Hi (Salut), Hey (Coucou), What's up? (Ça roule ?)", 'Dialogue': "Personnage A: Good morning, my name is John (Bonjour, je m'appelle John). Personnage B: Hi John, I'm Lisa (Salut John, je suis Lisa). Personnage A: Pleased to meet you (Enchanté). Personnage B: Nice to meet you too (Ravie de te rencontrer aussi).", 'Refrain (répété)': "Good morning (Bonjour), Hi (Salut), Hey (Coucou), What's up? (Ça roule ?)"}</t>
+          <t>{'Introduction': "Yo, écoute bien, on va apprendre,\nLes mots qu'il faut pour bien comprendre.\nFormel ou informel, c'est important,\nPour parler anglais, c'est le moment.", 'Refrain': "Formel ou informel, choisis bien tes mots,\nPour chaque situation, il y a le bon tempo.\n'Pleased to meet you' ou 'Hey, what’s up?',\nNavigue dans la langue, ne t'arrête pas.", 'Couplet': "Personnage A : Hello, my name is John (Bonjour, je m'appelle John).\nPersonnage B : Nice to meet you, John (Enchanté, John).\nPersonnage A : How do you do? (Comment ça va ?)\nPersonnage B : I'm doing well, thank you (Je vais bien, merci).\n\nPersonnage A : Hey, what's up? (Salut, ça roule ?)\nPersonnage B : Not much, just chilling (Pas grand-chose, je me détends).\nPersonnage A : How's it going? (Comment ça va ?)\nPersonnage B : It's going great, thanks (Ça va super, merci).\n\nPersonnage A : Good morning, sir (Bonjour, monsieur).\nPersonnage B : Good morning, how can I help you? (Bonjour, comment puis-je vous aider ?)\nPersonnage A : Could you open the window, please? (Pourriez-vous ouvrir la fenêtre, s'il vous plaît ?)\nPersonnage B : Of course, no problem (Bien sûr, pas de problème)."}</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn numbers, one to ten, \nApprenons les nombres, de un à dix.", 'Refrain': 'Count with me, one to ten, \nCompte avec moi, de un à dix.', 'Dialogue': "Personnage A: What's your favorite number? (Quel est ton nombre préféré?) \nPersonnage B: I like three (J'aime trois), it's 'thri' (c'est 'thri'). \nPersonnage A: I prefer seven (Je préfère sept), it's 'sevèn' (c'est 'sevèn'). \nPersonnage B: Let's count together (Comptons ensemble), one to ten (de un à dix)."}</t>
+          <t>{'Introduction': "Hey, let's learn to count, it's fun and easy (Hé, apprenons à compter, c'est amusant et facile).", 'Refrain': "One, two, three, four, five (Un, deux, trois, quatre, cinq),\nSix, seven, eight, nine, ten, let's thrive! (Six, sept, huit, neuf, dix, prospérons!)", 'Dialogue': "Personnage A: How do you say 'one' in English? (Comment dit-on 'un' en anglais?)\nPersonnage B: It's 'one' (C'est 'one').\nPersonnage A: And 'two'? (Et 'deux'?)\nPersonnage B: That's 'two' (C'est 'two').\nPersonnage A: What about 'three'? (Qu'en est-il de 'trois'?)\nPersonnage B: You say 'three' (Tu dis 'three').\nPersonnage A: Can you tell me 'four'? (Peux-tu me dire 'quatre'?)\nPersonnage B: Sure, it's 'four' (Bien sûr, c'est 'four').\nPersonnage A: And 'five'? (Et 'cinq'?)\nPersonnage B: It's 'five' (C'est 'five').\nPersonnage A: How do you say 'six'? (Comment dit-on 'six'?)\nPersonnage B: That's 'six' (C'est 'six').\nPersonnage A: And 'seven'? (Et 'sept'?)\nPersonnage B: It's 'seven' (C'est 'seven').\nPersonnage A: What about 'eight'? (Qu'en est-il de 'huit'?)\nPersonnage B: You say 'eight' (Tu dis 'eight').\nPersonnage A: Can you tell me 'nine'? (Peux-tu me dire 'neuf'?)\nPersonnage B: Sure, it's 'nine' (Bien sûr, c'est 'nine').\nPersonnage A: And 'ten'? (Et 'dix'?)\nPersonnage B: It's 'ten' (C'est 'ten')."}</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn numbers, eleven to twenty (Apprenons les nombres, onze à vingt)", 'Refrain': 'Eleven, twelve, thirteen, fourteen (Onze, douze, treize, quatorze), Fifteen, sixteen, seventeen, eighteen (Quinze, seize, dix-sept, dix-huit), Nineteen, twenty, count with me (Dix-neuf, vingt, compte avec moi)', 'Dialogue': "Personnage A: What's your favorite number? (Quel est ton nombre préféré?) Personnage B: It's fifteen, like my age! (C'est quinze, comme mon âge!) Personnage A: I have twelve apples. (J'ai douze pommes.) Personnage B: I need eighteen for the party. (J'ai besoin de dix-huit pour la fête.)"}</t>
+          <t>{'Introduction': "Hey, let's learn to count, from eleven to twenty, It's easy and fun, you'll see, plenty!", 'Refrain': "Thirteen, fourteen, fifteen, sixteen, (Treize, quatorze, quinze, seize,) Seventeen, eighteen, nineteen, a routine. (Dix-sept, dix-huit, dix-neuf, une routine.) End with twenty, a new decade, (Finis avec vingt, une nouvelle décennie,) Counting in English, you've got it made! (Compter en anglais, tu l'as réussi!)", 'Dialogue': "Personnage A: What's after ten? (Qu'est-ce qui vient après dix?) Personnage B: Eleven, it's unique, my friend. (Onze, c'est unique, mon ami.) Personnage A: And then? (Et ensuite?) Personnage B: Twelve, before we reach the teens. (Douze, avant d'atteindre les ados.) Personnage A: How do we say thirteen? (Comment dit-on treize?) Personnage B: Thirteen, with '-teen', it's keen. (Treize, avec '-teen', c'est astucieux.) Personnage A: What about fourteen? (Et quatorze?) Personnage B: Fourteen, just add '-teen'. (Quatorze, ajoute juste '-teen'.)"}</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to say our age in English! (Apprenons à dire notre âge en anglais !)", 'Refrain': "I am ... years old. (J'ai ... ans.)", 'Dialogue': "Personnage A: How old are you? (Quel âge as-tu ?) Personnage B: I am ten years old. (J'ai dix ans.) Personnage A: My brother is eight years old. (Mon frère a huit ans.) Personnage B: My sister is twelve years old. (Ma sœur a douze ans.)"}</t>
+          <t>{'Introduction': "Yo, apprendre à dire son âge en anglais, c'est facile, écoute ça !", 'Refrain': "I am [nombre] years old (J'ai [nombre] ans), c'est comme ça qu'on dit son âge.", 'Couplet': "Personnage A: Hey, how old are you? (Hé, quel âge as-tu ?)\nPersonnage B: I am ten years old (J'ai dix ans), et toi ?\nPersonnage A: I am twelve years old (J'ai douze ans), c'est cool !\nPersonnage B: My brother is twenty-one years old (Mon frère a vingt et un ans).\nPersonnage A: Wow, my sister is twenty-five years old (Wow, ma sœur a vingt-cinq ans) !", 'Conclusion': 'Pratique ces phrases, mémorise les nombres, et parle de ton âge facilement.'}</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to say your phone number in English (Apprenons à dire ton numéro de téléphone en anglais).", 'Refrain': 'Say each number clear and slow (Dis chaque chiffre clairement et lentement), practice makes you grow (la pratique te fait progresser).', 'Couplet sous forme de dialogue': "Personnage A: What's your number? (Quel est ton numéro?)\nPersonnage B: It's 123-456-7890 (C'est un deux trois, quatre cinq six, sept huit neuf zéro).\nPersonnage A: Oh, I see! (Ah, je vois!)\nPersonnage B: Yes, 'oh' for zero, easy! (Oui, 'oh' pour zéro, facile!)", 'Refrain (répété à l’identique)': 'Say each number clear and slow (Dis chaque chiffre clairement et lentement), practice makes you grow (la pratique te fait progresser).'}</t>
+          <t>{'Introduction': "Yo, apprenons à dire notre numéro de téléphone en anglais, c'est pratique et utile !", 'Refrain': 'One two three, four five six, seven eight nine zero. (Un deux trois, quatre cinq six, sept huit neuf zéro.)', 'Couplet 1': "Personnage A: What's your phone number? (Quel est ton numéro de téléphone ?)\nPersonnage B: It's three four five, six seven eight. (C'est trois quatre cinq, six sept huit.)\nPersonnage A: And the area code? (Et le code régional ?)\nPersonnage B: It's zero one two. (C'est zéro un deux.)", 'Couplet 2': "Personnage A: How do you say repeated numbers? (Comment dis-tu les chiffres répétés ?)\nPersonnage B: Use 'double', like double three. (Utilise 'double', comme double trois.)\nPersonnage A: So, double one is? (Donc, double un c'est ?)\nPersonnage B: Eleven! (Onze !)", 'Couplet 3': 'Personnage A: Can you give me an example? (Peux-tu me donner un exemple ?)\nPersonnage B: Sure, nine eight seven, six five four. (Bien sûr, neuf huit sept, six cinq quatre.)\nPersonnage A: And the last part? (Et la dernière partie ?)\nPersonnage B: Three two one zero. (Trois deux un zéro.)', 'Conclusion': 'Écoutez et répétez, améliorez votre prononciation et fluidité !'}</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>{'Introduction': "Découvre les dizaines en anglais, c'est facile et amusant !", 'Refrain': 'Twenty, thirty, forty, fifty (Vingt, trente, quarante, cinquante),\nSixty, seventy, eighty, ninety (Soixante, soixante-dix, quatre-vingts, quatre-vingt-dix).', 'Couplet sous forme de dialogue': "Personnage A: What's twenty in English? (Qu'est-ce que vingt en anglais?)\nPersonnage B: It's twenty, like twenty apples (C'est twenty, comme vingt pommes).\nPersonnage A: And thirty? (Et trente?)\nPersonnage B: Thirty, like thirty books (Thirty, comme trente livres).\nPersonnage A: How about forty? (Et quarante?)\nPersonnage B: Forty, like forty cars (Forty, comme quarante voitures).\nPersonnage A: Fifty? (Cinquante?)\nPersonnage B: Fifty, like fifty stars (Fifty, comme cinquante étoiles).", 'Refrain (répété à l’identique)': 'Twenty, thirty, forty, fifty (Vingt, trente, quarante, cinquante),\nSixty, seventy, eighty, ninety (Soixante, soixante-dix, quatre-vingts, quatre-vingt-dix).'}</t>
+          <t>{'Introduction': "Yo, écoute bien, on va compter, \nLes dizaines en anglais, c'est facile, tu vas voir!", 'Refrain': "Vingt, trente, quarante, cinquante, \nSoixante, soixante-dix, c'est excitant! \nQuatre-vingts, quatre-vingt-dix, cent, \nLes dizaines, c'est important!", 'Couplet': "Personnage A: Hey, do you know twenty (Vingt)? \nPersonnage B: Yes, twenty apples (Vingt pommes) in my bag. \nPersonnage A: And thirty (Trente), can you say it? \nPersonnage B: Thirty books (Trente livres) on the shelf, I see it! \nPersonnage A: What about forty (Quarante)? \nPersonnage B: Forty cars (Quarante voitures) on the street, that's plenty! \nPersonnage A: Fifty (Cinquante), do you know? \nPersonnage B: Fifty stars (Cinquante étoiles) in the sky, they glow!"}</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's count up, it's time to learn, \n(Comptons ensemble, il est temps d'apprendre,)", 'Refrain': "Count with me, twenty-one to fifty, \n(Compte avec moi, de vingt-et-un à cinquante,)\nFeel the beat, it's so nifty! \n(Ressens le rythme, c'est si astucieux!)", 'Dialogue': "Personnage A: What's your age? \n(Quel âge as-tu?)\nPersonnage B: I'm twenty-one. \n(J'ai vingt-et-un ans.)\nPersonnage A: How many apples? \n(Combien de pommes?)\nPersonnage B: I have thirty-five. \n(J'en ai trente-cinq.)\nPersonnage A: What's the time? \n(Quelle heure est-il?)\nPersonnage B: It's forty-two minutes past. \n(Il est quarante-deux minutes passées.)"}</t>
+          <t>{'Introduction': "Let's learn to count from twenty-one to fifty (Apprenons à compter de vingt et un à cinquante).", 'Refrain': "Count with me, let's go, from twenty-one to fifty, nice and slow (Compte avec moi, allons-y, de vingt et un à cinquante, doucement).", 'Dialogue': "Personnage A: How many apples do you have? (Combien de pommes as-tu?)\nPersonnage B: I have twenty-one apples (J'ai vingt et une pommes).\nPersonnage A: And how many oranges? (Et combien d'oranges?)\nPersonnage B: I have thirty oranges (J'ai trente oranges).\nPersonnage A: Can you count to forty? (Peux-tu compter jusqu'à quarante?)\nPersonnage B: Yes, thirty-one, thirty-two, thirty-three, up to forty (Oui, trente et un, trente-deux, trente-trois, jusqu'à quarante).\nPersonnage A: Great! How about forty-five? (Super ! Et quarante-cinq ?)\nPersonnage B: Forty-one, forty-two, forty-three, forty-four, forty-five (Quarante et un, quarante-deux, quarante-trois, quarante-quatre, quarante-cinq)."}</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's count up high, from fifty-one to the sky! (Comptons jusqu'au ciel, de cinquante et un au ciel!)", 'Refrain': 'Count with me, fifty-one to one hundred! (Compte avec moi, de cinquante et un à cent!)', 'Dialogue': "Personnage A: What's your number? (Quel est ton numéro?)\nPersonnage B: It's fifty-five! (C'est cinquante-cinq!)\nPersonnage A: Mine is sixty! (Le mien est soixante!)\nPersonnage B: Let's count together! (Comptons ensemble!)\nPersonnage A: Seventy-one, seventy-two! (Soixante et onze, soixante-douze!)\nPersonnage B: I like eighty-three! (J'aime quatre-vingt-trois!)\nPersonnage A: Ninety-nine is near! (Quatre-vingt-dix-neuf est proche!)\nPersonnage B: One hundred, we cheer! (Cent, on applaudit!)", 'Refrain (répété)': 'Count with me, fifty-one to one hundred! (Compte avec moi, de cinquante et un à cent!)'}</t>
+          <t>{'Introduction': "Let's learn to count, from fifty-one to one hundred, \nApprenons à compter, de cinquante et un à cent, \nIt's easy and fun, let's get started! \nC'est facile et amusant, commençons!", 'Refrain': "Count with me, from fifty-one to one hundred, \nCompte avec moi, de cinquante et un à cent, \nLearn the numbers, say them loud, \nApprends les chiffres, dis-les fort, \nPractice makes perfect, let's count out loud. \nLa pratique rend parfait, comptons à voix haute.", 'Dialogue': "Personnage A: What's your favorite number between fifty-one and sixty? \nQuel est ton chiffre préféré entre cinquante et un et soixante? \nPersonnage B: I like fifty-five (J'aime cinquante-cinq), it's easy to remember. \nC'est facile à retenir.\nPersonnage A: Can you count from sixty-one to seventy? \nPeux-tu compter de soixante et un à soixante-dix? \nPersonnage B: Sure! Sixty-one, sixty-two, sixty-three, sixty-four, sixty-five, sixty-six, sixty-seven, sixty-eight, sixty-nine, seventy. \nBien sûr! Soixante et un, soixante-deux, soixante-trois, soixante-quatre, soixante-cinq, soixante-six, soixante-sept, soixante-huit, soixante-neuf, soixante-dix.\nPersonnage A: Great! Now let's try from seventy-one to eighty. \nSuper! Maintenant essayons de soixante et onze à quatre-vingts. \nPersonnage B: Seventy-one, seventy-two, seventy-three, seventy-four, seventy-five, seventy-six, seventy-seven, seventy-eight, seventy-nine, eighty. \nSoixante et onze, soixante-douze, soixante-treize, soixante-quatorze, soixante-quinze, soixante-seize, soixante-dix-sept, soixante-dix-huit, soixante-dix-neuf, quatre-vingts."}</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's talk about prices (Parlons des prix).", 'Refrain': 'It costs... euros (Ça coûte... euros), say it clear (dis-le clairement).', 'Couplet': 'Personnage A: How much is this? (Combien ça coûte?)\nPersonnage B: It costs ten euros (Ça coûte dix euros).\nPersonnage A: And this one? (Et celui-ci?)\nPersonnage B: It costs twenty euros (Ça coûte vingt euros).'}</t>
+          <t>{'Introduction': "Let's learn to use numbers to talk about prices. (Apprenons à utiliser les nombres pour parler des prix.)", 'Refrain': 'It costs five euros, it costs ten euros, it costs twenty euros. (Ça coûte cinq euros, ça coûte dix euros, ça coûte vingt euros.)', 'Couplet': 'Person A: How much is this book? (Combien coûte ce livre ?)\nPerson B: It costs fifteen euros. (Ça coûte quinze euros.)\nPerson A: And this pen? (Et ce stylo ?)\nPerson B: It costs two euros. (Ça coûte deux euros.)\nPerson A: What about the notebook? (Et le cahier ?)\nPerson B: It costs three euros and fifty cents. (Ça coûte trois euros et cinquante centimes.)\nPerson A: How much for the backpack? (Combien pour le sac à dos ?)\nPerson B: It costs twenty-five euros. (Ça coûte vingt-cinq euros.)'}</t>
         </is>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn colors, red, blue, yellow! (Apprenons les couleurs, rouge, bleu, jaune!)", 'Refrain': 'Red, blue, yellow, colors we know! (Rouge, bleu, jaune, les couleurs que nous connaissons!)', 'Couplet sous forme de dialogue': "Personnage A: What's this apple's color? (Quelle est la couleur de cette pomme?)\nPersonnage B: It's red! (Elle est rouge!)\nPersonnage A: And the sky? (Et le ciel?)\nPersonnage B: It's blue! (Il est bleu!)\nPersonnage A: What about the sun? (Et le soleil?)\nPersonnage B: It's yellow! (Il est jaune!)"}</t>
+          <t>{'Introduction': "Let's learn colors, red, blue, yellow, it's fun! (Apprenons les couleurs, rouge, bleu, jaune, c'est amusant!)", 'Refrain': 'Red, blue, yellow, colors we see. (Rouge, bleu, jaune, couleurs que nous voyons.) Easy as one, two, three! (Facile comme un, deux, trois!)', 'Dialogue': "Personnage A: What color is the apple? (Quelle couleur est la pomme?)\nPersonnage B: It's red, like a fire truck! (Elle est rouge, comme un camion de pompiers!)\nPersonnage A: And the sky, what color is it? (Et le ciel, de quelle couleur est-il?)\nPersonnage B: It's blue, like the ocean! (Il est bleu, comme l'océan!)\nPersonnage A: What about the banana? (Et la banane?)\nPersonnage B: It's yellow, like the sun! (Elle est jaune, comme le soleil!)"}</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn colors with objects, it's fun and easy! (Apprenons les couleurs avec des objets, c'est amusant et facile!)", 'Refrain': 'Colors, colors, everywhere we see! (Couleurs, couleurs, partout où nous voyons!)', 'Dialogue': "Personnage A: The apple is red (La pomme est rouge). Personnage B: Yes, and the banana is yellow (Oui, et la banane est jaune). Personnage A: The sky is blue (Le ciel est bleu). Personnage B: And the grass is green (Et l'herbe est verte). Personnage A: The orange is orange (L'orange est orange). Personnage B: The cat is black (Le chat est noir). Personnage A: The snow is white (La neige est blanche). Personnage B: And the chocolate is brown (Et le chocolat est marron). Personnage A: The flower is pink (La fleur est rose). Personnage B: The grape is purple (Le raisin est violet).", 'Refrain (répété)': 'Colors, colors, everywhere we see! (Couleurs, couleurs, partout où nous voyons!)'}</t>
+          <t>{'Introduction': "Yo, let's learn colors, it's easy and fun (Yo, apprenons les couleurs, c'est facile et amusant)", 'Refrain': 'Colors everywhere, in all that we see (Les couleurs partout, dans tout ce que nous voyons)\nRed, blue, yellow, green, learn them with me (Rouge, bleu, jaune, vert, apprends-les avec moi)', 'Dialogue': "Personnage A: What's the color of the apple? (Quelle est la couleur de la pomme?)\nPersonnage B: The apple is red, can't you see? (La pomme est rouge, tu ne vois pas?)\nPersonnage A: And the sky above us? (Et le ciel au-dessus de nous?)\nPersonnage B: The sky is blue, so high and free. (Le ciel est bleu, si haut et libre)\nPersonnage A: What about the banana? (Et la banane?)\nPersonnage B: The banana is yellow, bright as can be. (La banane est jaune, aussi brillante que possible)\nPersonnage A: And the grass under our feet? (Et l'herbe sous nos pieds?)\nPersonnage B: The grass is green, like a leafy sea. (L'herbe est verte, comme une mer feuillue)"}</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>{'Introduction': 'Apprenons les couleurs pour décrire les vêtements !', 'Refrain': "Il/Elle porte un pull bleu (He/She wears a blue sweater),\nUne robe rouge (A red dress), c'est facile à dire !", 'Couplet': 'Personnage A: What color is your shirt? (Quelle couleur est ta chemise ?)\nPersonnage B: My shirt is green (Ma chemise est verte).\nPersonnage A: And your pants? (Et ton pantalon ?)\nPersonnage B: My pants are brown (Mon pantalon est marron).'}</t>
+          <t>{'Introduction': "Yo, écoute bien, on va apprendre,\nLes couleurs et les vêtements, c'est le plan.", 'Refrain': "Il/Elle porte, c'est facile à dire,\nUn vêtement coloré, à décrire.\nPratique chaque jour, avec passion,\nLes couleurs et les vêtements, en toute saison.", 'Couplet': 'Personnage A: What color is your shirt? (De quelle couleur est ta chemise?)\nPersonnage B: My shirt is red. (Ma chemise est rouge.)\nPersonnage A: And your pants? (Et ton pantalon?)\nPersonnage B: They are black. (Ils sont noirs.)\nPersonnage A: What about your shoes? (Et tes chaussures?)\nPersonnage B: My shoes are white. (Mes chaussures sont blanches.)\nPersonnage A: Is your hat blue? (Ton chapeau est-il bleu?)\nPersonnage B: Yes, it is blue. (Oui, il est bleu.)'}</t>
         </is>
       </c>
     </row>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>{'Introduction': 'Yo, apprenons les jours de la semaine !', 'Refrain': 'Monday, Tuesday, Wednesday, (Lundi, Mardi, Mercredi), Thursday, Friday, Saturday, Sunday! (Jeudi, Vendredi, Samedi, Dimanche!)', 'Couplet sous forme de dialogue': "Personnage A: What's today? (Quel jour sommes-nous?) Personnage B: It's Monday! (C'est lundi!) Personnage A: Let's meet on Tuesday. (Rendez-vous mardi.) Personnage B: Sure, see you Wednesday! (Bien sûr, à mercredi!)", 'Refrain (répété à l’identique)': 'Monday, Tuesday, Wednesday, (Lundi, Mardi, Mercredi), Thursday, Friday, Saturday, Sunday! (Jeudi, Vendredi, Samedi, Dimanche!)'}</t>
+          <t>{'Introduction': "Yo, écoute bien, on va apprendre les jours, en anglais et en français, c'est parti !", 'Refrain': 'Monday, Tuesday, Wednesday, Thursday, Friday, Saturday, Sunday. (Lundi, mardi, mercredi, jeudi, vendredi, samedi, dimanche.)', 'Couplet': "Personnage A: What's today? (Quel jour sommes-nous ?) Personnage B: Today is Monday. (Aujourd'hui c'est lundi.) Personnage A: And tomorrow? (Et demain ?) Personnage B: Tomorrow is Tuesday. (Demain c'est mardi.) Personnage A: What about yesterday? (Et hier ?) Personnage B: Yesterday was Sunday. (Hier c'était dimanche.) Personnage A: What's your favorite day? (Quel est ton jour préféré ?) Personnage B: I love Saturday! (J'adore le samedi !)"}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor music lyrics parsing and structure; enhance data models and improve error handling
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dire son nom</t>
+          <t>Se saluer et prendre congé (formel / informel)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>apprendre à dire son nom  ("Je m'appelle...") en anglais</t>
+          <t>Apprendre à dire bonjour et au revoir dans des contextes formels et informels (ex : Hola, ¿Qué tal?, Adiós, Hasta luego).</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'Introduction': "Hello! My name is... (Bonjour ! Je m'appelle...)", 'Refrain': "What's your name? Nice to meet you! (Quel est ton nom ? Enchanté de te rencontrer !)", 'Couplet': "Personnage A: Hi! I'm Anna. (Salut ! Je m'appelle Anna.)\nPersonnage B: Nice to meet you, Anna. I'm Tom. (Enchanté de te rencontrer, Anna. Je m'appelle Tom.)\nPersonnage A: What's your name? (Quel est ton nom ?)\nPersonnage B: My name is Tom. (Je m'appelle Tom.)\nPersonnage A: Pleased to meet you, Tom. (Ravi de te rencontrer, Tom.)\nPersonnage B: Let's start a conversation. (Commençons une conversation.)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprender a saludar y despedirse en español es esencial. (Apprendre à saluer et à prendre congé en espagnol est essentiel.)', 'Aquí tienes algunas expresiones básicas para un nivel A1. (Voici quelques expressions de base pour un niveau A1.)']) refrain_1=LyricsSection(lines=['Hola - Salut', '¿Qué tal? - Comment ça va ?', '¿Cómo estás? - Comment vas-tu ?', '¿Qué pasa? - Quoi de neuf ?']) couplet=LyricsSection(lines=['A: Buenos días, ¿cómo estás? (Bonjour, comment vas-tu ?)', 'B: Muy bien, gracias. ¿Y tú? (Très bien, merci. Et toi ?)', 'A: Bien también, gracias. (Bien aussi, merci.)', 'B: ¿Qué tal tu día? (Comment se passe ta journée ?)', 'A: Todo bien, gracias. (Tout va bien, merci.)']) refrain_2=LyricsSection(lines=['Hola - Salut', '¿Qué tal? - Comment ça va ?', '¿Cómo estás? - Comment vas-tu ?', '¿Qué pasa? - Quoi de neuf ?']) mini_dialogue=LyricsSection(lines=['A: Hasta mañana. (À demain.)', 'B: Hasta pronto. (À bientôt.)', 'A: Que tenga un buen día. (Passez une bonne journée.)', 'B: Fue un placer. (Ce fut un plaisir.)']) outro=LyricsSection(lines=['Estas expresiones te ayudarán a interactuar de manera adecuada. (Ces expressions vous aideront à interagir de manière appropriée.)', "¡Buena suerte con tu aprendizaje del español! (Bonne chance avec votre apprentissage de l'espagnol !)"])</t>
         </is>
       </c>
     </row>
@@ -521,12 +521,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dire son âge</t>
+          <t>Donner son nom, prénom, nationalité</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>apprendre à dire son âge  ("J'ai ... ans.") en anglais</t>
+          <t>Apprendre à se présenter avec son prénom, nom, et nationalité (ex : Me llamo..., Soy de..., Soy francés/francesa).</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -536,12 +536,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, listen up, it's time to engage, We're learning how to say our age!", 'Refrain': "I am five years old (J'ai cinq ans), I am ten years old (J'ai dix ans), Use 'I am' and numbers (Utilise 'I am' et les chiffres), that's how it's told (c'est comme ça qu'on le dit).", 'Dialogue': "Personnage A: Hey, how old are you? (Hé, quel âge as-tu ?) Personnage B: I am seven years old (J'ai sept ans), how about you? (et toi ?) Personnage A: I am eight years old (J'ai huit ans), that's cool, right? (c'est cool, non ?) Personnage B: Yeah, my sister is nine (Oui, ma sœur a neuf ans), she's out of sight! (elle est géniale !) Personnage A: My brother is ten (Mon frère a dix ans), he's really tall (il est vraiment grand). Personnage B: Wow, that's great! (Waouh, c'est super !) Let's learn them all! (Apprenons-les tous !)"}</t>
+          <t>introduction=LyricsSection(lines=['Hola, me llamo [tu nombre].', "Bonjour, je m'appelle [ton prénom]."]) refrain_1=LyricsSection(lines=['Mi apellido es [tu apellido].', 'Mon nom de famille est [ton nom de famille].']) couplet=LyricsSection(lines=['A: Hola, ¿cómo te llamas?', "A: Bonjour, comment tu t'appelles ?", 'B: Me llamo Ana. ¿Y tú?', "B: Je m'appelle Ana. Et toi ?", 'A: Me llamo Carlos.', "A: Je m'appelle Carlos.", 'B: ¿De dónde eres?', "B: D'où viens-tu ?", 'A: Soy de México. ¿Y tú?', 'A: Je viens du Mexique. Et toi ?', 'B: Soy de Argentina.', "B: Je viens d'Argentine."]) refrain_2=LyricsSection(lines=['Mi apellido es [tu apellido].', 'Mon nom de famille est [ton nom de famille].']) mini_dialogue=LyricsSection(lines=['Hola, me llamo Juan. Mi apellido es Pérez. Soy español. Soy de España.', "Bonjour, je m'appelle Juan. Mon nom de famille est Pérez. Je suis espagnol. Je viens d'Espagne."]) outro=LyricsSection(lines=["N'hésite pas à pratiquer ces phrases pour te sentir plus à l'aise lors de tes présentations en espagnol !", 'No dudes en practicar estas frases para sentirte más cómodo al presentarte en español.'])</t>
         </is>
       </c>
     </row>
@@ -561,12 +561,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dire sa nationalité </t>
+          <t>Dire son âge, sa date de naissance</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>apprendre à dire sa nationalité ("Je suis ...") en anglais</t>
+          <t>Apprendre à dire son âge et sa date de naissance (ex : Tengo ... años, Nací el...).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -576,12 +576,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, let's learn how to say your nationality, (Yo, apprenons à dire ta nationalité,) in English, it's easy, you'll see! (en anglais, c'est facile, tu verras!)", 'Refrain': "I am [nationality], that's the way to say, (Je suis [nationalité], c'est comme ça qu'on dit,) 'I am French', 'I am American', every day! (Je suis Français, Je suis Américain, chaque jour!)", 'Couplet': "Personnage A: Hey, what's your name? (Hé, comment tu t'appelles?)\nPersonnage B: My name is Anna, and I am Italian. (Je m'appelle Anna, et je suis Italienne.)\nPersonnage A: Cool! I am John, and I am Canadian. (Cool! Je m'appelle John, et je suis Canadien.)\nPersonnage B: Nice to meet you, John! (Enchantée de te rencontrer, John!)\nPersonnage A: Likewise, Anna! (Moi de même, Anna!)", 'Outro': "With practice, you'll express your nationality, (Avec de la pratique, tu exprimeras ta nationalité,) simply and clearly, that's the key! (simplement et clairement, c'est la clé!)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprendamos a decir nuestra edad y fecha de nacimiento.', 'Apprenons à dire notre âge et notre date de naissance.']) refrain_1=LyricsSection(lines=['Tengo [nombre] años.', "J'ai [nombre] ans."]) couplet=LyricsSection(lines=['A: ¿Cuántos años tienes?', 'A: Quel âge as-tu?', 'B: Tengo 20 años.', "B: J'ai 20 ans.", 'A: ¿Cuándo naciste?', 'A: Quand es-tu né?', 'B: Nací el 15 de marzo de 2003.', 'B: Je suis né le 15 mars 2003.', 'A: ¡Qué interesante!', "A: C'est intéressant!"]) refrain_2=LyricsSection(lines=['Tengo [nombre] años.', "J'ai [nombre] ans."]) mini_dialogue=LyricsSection(lines=['¿Cuántos años tienes? Tengo 20 años.', "Quel âge as-tu? J'ai 20 ans."]) outro=LyricsSection(lines=['¡Buena suerte con tu aprendizaje del español!', "Bonne chance avec ton apprentissage de l'espagnol !"])</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Poser des questions</t>
+          <t>Dire où l’on habite</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>apprendre à poser des questions pour demander le nom et l'âge ("Comment tu t'appelles ?", "Quel âge as-tu ?")</t>
+          <t>Apprendre à dire où on habite et décrire simplement son lieu de vie (ex : Vivo en Madrid, Vivo en una casa).</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">anglais </t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, apprendre à poser des questions, c'est essentiel (important).", 'Refrain': "Répète et pratique, pour t'améliorer chaque jour (every day).", 'Couplet': "Personnage A: Hey, what's your name? (Comment tu t'appelles ?)\nPersonnage B: My name is Anna (Je m'appelle Anna).\nPersonnage A: Nice to meet you, Anna (Enchanté, Anna).\nPersonnage A: How old are you? (Quel âge as-tu ?)\nPersonnage B: I'm ten years old (J'ai dix ans).\nPersonnage A: Cool, let's play! (Super, jouons !)\nPersonnage A: What's your favorite color? (Quelle est ta couleur préférée ?)\nPersonnage B: Blue, like the sky (Bleu, comme le ciel).\nPersonnage A: Great choice! (Bon choix !)", 'Conclusion': "Avec la pratique, tu seras à l'aise pour poser ces questions (questions)."}</t>
+          <t>introduction=LyricsSection(lines=["Para aprender a decir dónde vives en español, aquí hay algunas frases básicas. (Pour apprendre à dire où l'on habite en espagnol, voici quelques phrases de base.)"]) refrain_1=LyricsSection(lines=['Vivo en Madrid. (Je vis à Madrid.)', 'Vivo en Barcelona. (Je vis à Barcelone.)', 'Vivo en España. (Je vis en Espagne.)']) couplet=LyricsSection(lines=['A: ¿Dónde vives? (Où habites-tu ?)', 'B: Vivo en una casa. (Je vis dans une maison.)', 'A: ¿Es grande tu casa? (Ta maison est-elle grande ?)', 'B: Sí, mi casa es grande. (Oui, ma maison est grande.)', 'A: ¿Vives con tu familia? (Vis-tu avec ta famille ?)', 'B: Sí, vivo con mi familia. (Oui, je vis avec ma famille.)']) refrain_2=LyricsSection(lines=['Vivo en Madrid. (Je vis à Madrid.)', 'Vivo en Barcelona. (Je vis à Barcelone.)', 'Vivo en España. (Je vis en Espagne.)']) mini_dialogue=LyricsSection(lines=['Mi casa es grande. (Ma maison est grande.)', 'Mi apartamento es pequeño. (Mon appartement est petit.)', 'Mi piso tiene dos habitaciones. (Mon appartement a deux chambres.)', 'Mi casa tiene un jardín. (Ma maison a un jardin.)']) outro=LyricsSection(lines=['Vivo con mi familia. (Je vis avec ma famille.)', 'Vivo con amigos. (Je vis avec des amis.)', 'Vivo solo/sola. (Je vis seul/seule.)'])</t>
         </is>
       </c>
     </row>
@@ -641,12 +641,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dire où on habite </t>
+          <t>Parler de sa langue maternelle / des langues parlées</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>apprendre à dire où on habite ("J'habite à ...") en anglais</t>
+          <t>Apprendre à parler des langues qu’on parle (ex : Hablo francés y un poco de español).</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, let's learn how to say where you live, it's a basic skill, let's give it a spin!", 'Refrain': "I live in Paris (J'habite à Paris), I live in France (J'habite en France), I live in New York (J'habite à New York), I live in the United States (J'habite aux États-Unis).", 'Dialogue': "Personnage A: Hey, where do you live? (Hé, où habites-tu?)\nPersonnage B: I live in London. (J'habite à Londres.)\nPersonnage A: Oh cool, I live in a small town. (Oh cool, j'habite dans une petite ville.)\nPersonnage B: Do you like it there? (Aimes-tu là-bas?)\nPersonnage A: Yes, it's nice. I live in the countryside. (Oui, c'est sympa. J'habite à la campagne.)\nPersonnage B: I live in the capital city. (J'habite dans la capitale.)\nPersonnage A: That's exciting! (C'est excitant!)"}</t>
+          <t>introduction=LyricsSection(lines=['Mi lengua materna es el francés. (Ma langue maternelle est le français.)', 'Hablo francés. (Je parle français.)']) refrain_1=LyricsSection(lines=['Hablo un poco de español. (Je parle un peu espagnol.)', 'Hablo inglés y francés. (Je parle anglais et français.)']) couplet=LyricsSection(lines=["A: Estoy aprendiendo español. (A: J'apprends l'espagnol.)", 'B: ¿Qué lenguas hablas? (B: Quelles langues parles-tu ?)', "A: Hablo inglés y un poco de español. (A: Je parle anglais et un peu d'espagnol.)", 'B: ¿Hablas francés también? (B: Parles-tu aussi français ?)', 'A: Sí, hablo francés. (A: Oui, je parle français.)']) refrain_2=LyricsSection(lines=['Hablo un poco de español. (Je parle un peu espagnol.)', 'Hablo inglés y francés. (Je parle anglais et français.)']) mini_dialogue=LyricsSection(lines=['A: No, no hablo alemán. (A: Non, je ne parle pas allemand.)', 'B: Hablo español a nivel básico. (B: Je parle espagnol à un niveau basique.)']) outro=LyricsSection(lines=['Hablo francés con fluidez. (Je parle français couramment.)'])</t>
         </is>
       </c>
     </row>
@@ -681,12 +681,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dire au revoir</t>
+          <t>L’alphabet espagnol : épeler son nom</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>apprendre à Dire au revoir ("Au revoir", "À bientôt", "Bonne journée") en anglais</t>
+          <t>Apprendre à épeler son prénom et son nom avec l’alphabet espagnol (ex : Mi nombre se escribe...).</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to say goodbye (au revoir) in English, it's easy and fun!", 'Refrain': 'Goodbye, see you soon (À bientôt), Take care, have a nice afternoon (Bonne après-midi).', 'Dialogue': "Personnage A: Hey, it's time to go. Goodbye! (Hé, il est temps de partir. Au revoir!)\nPersonnage B: Goodbye! See you tomorrow! (Au revoir! À demain!)\nPersonnage A: I'm leaving now. Take care! (Je pars maintenant. Prends soin de toi!)\nPersonnage B: You too, have a nice day! (Toi aussi, passe une bonne journée!)\nPersonnage A: Bye, catch you later! (Salut, à plus tard!)\nPersonnage B: Later! Have a good one! (À plus! Bonne journée!)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprender a deletrear tu nombre en español es una habilidad básica muy útil.', '(Apprendre à épeler son nom en espagnol est une compétence de base très utile.)', 'Aquí te mostramos cómo puedes deletrear tu nombre y apellido usando el alfabeto español.', "(Voici comment vous pouvez épeler votre prénom et votre nom en utilisant l'alphabet espagnol.)"]) refrain_1=LyricsSection(lines=['Mi nombre se escribe A-N-A.', "(Mon prénom s'écrit A-N-A.)", 'A (a)', '(A)', 'N (ene)', '(N)', 'A (a)', '(A)']) couplet=LyricsSection(lines=['A: ¿Cómo se escribe tu apellido?', "(A: Comment s'écrit ton nom de famille ?)", 'B: Mi apellido se escribe G-A-R-C-Í-A.', "(B: Mon nom de famille s'écrit G-A-R-C-Í-A.)", 'A: G (ge)', '(A: G)', 'B: A (a)', '(B: A)', 'A: R (erre)', '(A: R)', 'B: C (ce)', '(B: C)', 'A: Í (i con acento)', '(A: Í)', 'B: A (a)', '(B: A)']) refrain_2=LyricsSection(lines=['Mi nombre se escribe A-N-A.', "(Mon prénom s'écrit A-N-A.)", 'A (a)', '(A)', 'N (ene)', '(N)', 'A (a)', '(A)']) mini_dialogue=LyricsSection(lines=["No olvides mencionar los acentos si tu nombre los tiene, como en 'García'.", "(N'oubliez pas de mentionner les accents si votre nom en contient, comme dans 'García'.)"]) outro=LyricsSection(lines=['¡Ahora puedes intentar deletrear tu propio nombre usando esta guía!', "(Vous pouvez maintenant essayer d'épeler votre propre nom en utilisant ce guide !)"])</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Utiliser des expressions de politesse</t>
+          <t>Compter de 1 à 20</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>apprendre à Utiliser des expressions de politesse ("Merci", "S'il vous plaît")</t>
+          <t>Apprendre à compter de 1 à 20 en espagnol (ex : uno, dos, tres... veinte).</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -736,12 +736,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, apprenons les mots de politesse, c'est essentiel pour l'anglais, pas de stress.", 'Refrain': 'La politesse est la clé, dans chaque interaction, en anglais comme ailleurs.', 'Dialogue': "Personnage A: Hey, could you pass the salt, please? (Hé, pourrais-tu passer le sel, s'il te plaît?)\nPersonnage B: Sure, here you go. Thank you for asking! (Bien sûr, voilà. Merci d'avoir demandé!)\nPersonnage A: You're welcome! (De rien!)\nPersonnage B: Excuse me, do you have the time? (Excusez-moi, avez-vous l'heure?)\nPersonnage A: Sorry, I don't have a watch. (Désolé, je n'ai pas de montre.)\nPersonnage B: No problem, thanks anyway! (Pas de problème, merci quand même!)\nPersonnage A: May I sit here? (Puis-je m'asseoir ici?)\nPersonnage B: Yes, please do. (Oui, je vous en prie.)", 'Conclusion': 'Pratiquez ces expressions, et la politesse sera votre alliée.'}</t>
+          <t>introduction=LyricsSection(lines=['¡Vamos a contar en español!', '(Allons compter en espagnol !)']) refrain_1=LyricsSection(lines=['Uno, dos, tres, cuatro, cinco,', '(Un, deux, trois, quatre, cinq,)', 'Seis, siete, ocho, nueve, diez.', '(Six, sept, huit, neuf, dix.)']) couplet=LyricsSection(lines=['A: ¿Cuántos dedos tienes en una mano?', '(A: Combien de doigts as-tu sur une main ?)', 'B: Tengo cinco dedos, mira bien.', "(B: J'ai cinq doigts, regarde bien.)", 'A: ¿Y en las dos manos?', '(A: Et sur les deux mains ?)', 'B: Diez en total, fácil de ver.', '(B: Dix en tout, facile à voir.)', 'A: ¿Puedes contar hasta veinte?', "(A: Peux-tu compter jusqu'à vingt ?)", 'B: Claro que sí, escucha bien.', '(B: Bien sûr, écoute bien.)']) refrain_2=LyricsSection(lines=['Uno, dos, tres, cuatro, cinco,', '(Un, deux, trois, quatre, cinq,)', 'Seis, siete, ocho, nueve, diez.', '(Six, sept, huit, neuf, dix.)']) mini_dialogue=LyricsSection(lines=['A: ¿Y después del diez?', '(A: Et après dix ?)', 'B: Once, doce, trece, catorce, quince.', '(B: Onze, douze, treize, quatorze, quinze.)']) outro=LyricsSection(lines=['Dieciséis, diecisiete, dieciocho, diecinueve, veinte.', '(Seize, dix-sept, dix-huit, dix-neuf, vingt.)', '¡Bien hecho, ya sabes contar!', '(Bien joué, tu sais maintenant compter !)'])</t>
         </is>
       </c>
     </row>
@@ -761,12 +761,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Répondre à "Comment ça va ?" </t>
+          <t>Se présenter à l’écrit (mini-biographie simple)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>apprendre à Répondre à "Comment ça va ?" ("Ça va bien", "Pas mal", "Ça va mal")</t>
+          <t>Apprendre à écrire une courte présentation personnelle (nom, âge, nationalité, ville).</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -776,12 +776,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, apprenons à répondre à 'Comment ça va ?' en anglais, c'est essentiel (Yo, apprenons à répondre à 'Comment ça va ?' en anglais, c'est essentiel).", 'Refrain': "Exprime tes sentiments, avec le bon ton, c'est important (Exprime tes sentiments, avec le bon ton, c'est important).", 'Couplet 1': "Personnage A: Hey, how are you? (Hey, comment ça va ?)\nPersonnage B: I'm good, thanks! (Ça va bien, merci !)\nPersonnage A: How's your day? (Comment se passe ta journée ?)\nPersonnage B: I'm fine, just working. (Ça va, je travaille juste.)\nPersonnage A: Feeling well today? (Tu te sens bien aujourd'hui ?)\nPersonnage B: Yes, I'm well, and you? (Oui, je vais bien, et toi ?)", 'Couplet 2': "Personnage A: How are things? (Comment ça va ?)\nPersonnage B: Not bad, just a bit tired. (Pas mal, juste un peu fatigué.)\nPersonnage A: Are you okay? (Ça va ?)\nPersonnage B: I'm okay, just busy. (Ça va, juste occupé.)\nPersonnage A: Everything alright? (Tout va bien ?)\nPersonnage B: I'm alright, thanks for asking. (Ça va, merci de demander.)", 'Couplet 3': "Personnage A: How are you feeling? (Comment te sens-tu ?)\nPersonnage B: I'm not so good, a bit sick. (Je ne vais pas très bien, un peu malade.)\nPersonnage A: Anything wrong? (Quelque chose ne va pas ?)\nPersonnage B: I'm not great, had a rough day. (Je ne vais pas bien, j'ai eu une journée difficile.)\nPersonnage A: Need any help? (Besoin d'aide ?)\nPersonnage B: I'm not well, but I'll manage. (Je ne vais pas bien, mais je vais gérer.)", 'Conclusion': 'Ces phrases simples te guideront dans chaque conversation (Ces phrases simples te guideront dans chaque conversation).'}</t>
+          <t>introduction=LyricsSection(lines=['Hola, vamos a aprender a presentarnos en español.', '(Bonjour, nous allons apprendre à nous présenter en espagnol.)']) refrain_1=LyricsSection(lines=['Me llamo [Tu Nombre]. Tengo [Tu Edad] años.', "(Je m'appelle [Ton Nom]. J'ai [Ton Âge] ans.)", 'Soy [Tu Nacionalidad]. Vivo en [Tu Ciudad].', "(Je suis [Ta Nationalité]. J'habite à [Ta Ville].)"]) couplet=LyricsSection(lines=['A: Hola, ¿cómo te llamas?', "(A: Bonjour, comment tu t'appelles ?)", 'B: Me llamo Ana. ¿Y tú?', "(B: Je m'appelle Ana. Et toi ?)", 'A: Me llamo Juan. ¿Cuántos años tienes?', "(A: Je m'appelle Juan. Quel âge as-tu ?)", 'B: Tengo 20 años. ¿Y tú?', "(B: J'ai 20 ans. Et toi ?)", 'A: Tengo 22 años. ¿De dónde eres?', "(A: J'ai 22 ans. D'où viens-tu ?)", 'B: Soy francesa. Vivo en París.', "(B: Je suis française. J'habite à Paris.)"]) refrain_2=LyricsSection(lines=['Me llamo [Tu Nombre]. Tengo [Tu Edad] años.', "(Je m'appelle [Ton Nom]. J'ai [Ton Âge] ans.)", 'Soy [Tu Nacionalidad]. Vivo en [Tu Ciudad].', "(Je suis [Ta Nationalité]. J'habite à [Ta Ville].)"]) mini_dialogue=LyricsSection(lines=['A: ¿Qué te gusta hacer?', "(A: Qu'aimes-tu faire ?)", 'B: Me gusta leer.', "(B: J'aime lire.)"]) outro=LyricsSection(lines=['Ahora sabes presentarte en español. ¡Bien hecho!', '(Maintenant tu sais te présenter en espagnol. Bien joué !)'])</t>
         </is>
       </c>
     </row>
@@ -801,12 +801,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Expressions pour des situations formelles et informelles</t>
+          <t>Poser des questions personnelles simples à quelqu’un; Parler de sa famille : membres, âge, prénoms</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>apprendre les Expressions pour des situations formelles et informelles ("Enchanté(e)", "Ça roule ?")</t>
+          <t>Apprendre à poser des questions simples et à parler de sa famille (ex : ¿Tienes hermanos?, Mi madre se llama...).</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -816,12 +816,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, écoute bien, on va apprendre,\nLes mots qu'il faut pour bien comprendre.\nFormel ou informel, c'est important,\nPour parler anglais, c'est le moment.", 'Refrain': "Formel ou informel, choisis bien tes mots,\nPour chaque situation, il y a le bon tempo.\n'Pleased to meet you' ou 'Hey, what’s up?',\nNavigue dans la langue, ne t'arrête pas.", 'Couplet': "Personnage A : Hello, my name is John (Bonjour, je m'appelle John).\nPersonnage B : Nice to meet you, John (Enchanté, John).\nPersonnage A : How do you do? (Comment ça va ?)\nPersonnage B : I'm doing well, thank you (Je vais bien, merci).\n\nPersonnage A : Hey, what's up? (Salut, ça roule ?)\nPersonnage B : Not much, just chilling (Pas grand-chose, je me détends).\nPersonnage A : How's it going? (Comment ça va ?)\nPersonnage B : It's going great, thanks (Ça va super, merci).\n\nPersonnage A : Good morning, sir (Bonjour, monsieur).\nPersonnage B : Good morning, how can I help you? (Bonjour, comment puis-je vous aider ?)\nPersonnage A : Could you open the window, please? (Pourriez-vous ouvrir la fenêtre, s'il vous plaît ?)\nPersonnage B : Of course, no problem (Bien sûr, pas de problème)."}</t>
+          <t>introduction=LyricsSection(lines=['Aprender a hablar de tu familia en español es un buen comienzo. (Apprendre à parler de ta famille en espagnol est un bon début.)']) refrain_1=LyricsSection(lines=['¿Tienes hermanos? (As-tu des frères et sœurs ?)', "¿Cómo se llaman tus padres? (Comment s'appellent tes parents ?)", '¿Cuántos años tiene tu hermano? (Quel âge a ton frère ?)']) couplet=LyricsSection(lines=['A: Hola, ¿tienes hermanos? (Salut, as-tu des frères et sœurs ?)', "B: Sí, tengo dos hermanos. (Oui, j'ai deux frères.)", "A: ¿Cómo se llama tu madre? (Comment s'appelle ta mère ?)", "B: Mi madre se llama Ana. (Ma mère s'appelle Ana.)", 'A: ¿Y tu padre? (Et ton père ?)', "B: Mi padre se llama Juan y tiene 50 años. (Mon père s'appelle Juan et il a 50 ans.)"]) refrain_2=LyricsSection(lines=['¿Tienes hermanos? (As-tu des frères et sœurs ?)', "¿Cómo se llaman tus padres? (Comment s'appellent tes parents ?)", '¿Cuántos años tiene tu hermano? (Quel âge a ton frère ?)']) mini_dialogue=LyricsSection(lines=['A: ¿Tu familia es grande o pequeña? (Ta famille est-elle grande ou petite ?)', "B: Es grande, mis primos son de España. (Elle est grande, mes cousins sont d'Espagne.)"]) outro=LyricsSection(lines=['Practica estas frases y conocerás mejor a la gente. ¡Buena suerte! (Pratique ces phrases et tu connaîtras mieux les gens. Bonne chance !)'])</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Apprendre les nombres de 1 à 10</t>
+          <t>Décrire une personne (physique)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">comment dire 1 à 10 en anglais </t>
+          <t>Apprendre à décrire le physique d’une personne (cheveux, taille, vêtements) avec des adjectifs simples.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -856,12 +856,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>{'Introduction': "Hey, let's learn to count, it's fun and easy (Hé, apprenons à compter, c'est amusant et facile).", 'Refrain': "One, two, three, four, five (Un, deux, trois, quatre, cinq),\nSix, seven, eight, nine, ten, let's thrive! (Six, sept, huit, neuf, dix, prospérons!)", 'Dialogue': "Personnage A: How do you say 'one' in English? (Comment dit-on 'un' en anglais?)\nPersonnage B: It's 'one' (C'est 'one').\nPersonnage A: And 'two'? (Et 'deux'?)\nPersonnage B: That's 'two' (C'est 'two').\nPersonnage A: What about 'three'? (Qu'en est-il de 'trois'?)\nPersonnage B: You say 'three' (Tu dis 'three').\nPersonnage A: Can you tell me 'four'? (Peux-tu me dire 'quatre'?)\nPersonnage B: Sure, it's 'four' (Bien sûr, c'est 'four').\nPersonnage A: And 'five'? (Et 'cinq'?)\nPersonnage B: It's 'five' (C'est 'five').\nPersonnage A: How do you say 'six'? (Comment dit-on 'six'?)\nPersonnage B: That's 'six' (C'est 'six').\nPersonnage A: And 'seven'? (Et 'sept'?)\nPersonnage B: It's 'seven' (C'est 'seven').\nPersonnage A: What about 'eight'? (Qu'en est-il de 'huit'?)\nPersonnage B: You say 'eight' (Tu dis 'eight').\nPersonnage A: Can you tell me 'nine'? (Peux-tu me dire 'neuf'?)\nPersonnage B: Sure, it's 'nine' (Bien sûr, c'est 'nine').\nPersonnage A: And 'ten'? (Et 'dix'?)\nPersonnage B: It's 'ten' (C'est 'ten')."}</t>
+          <t>introduction=LyricsSection(lines=['Vamos a aprender a describir a una persona. (Nous allons apprendre à décrire une personne.)']) refrain_1=LyricsSection(lines=['Cheveux (Pelo) :', 'Pelo largo (cheveux longs), Pelo corto (cheveux courts), Pelo rizado (cheveux bouclés), Pelo liso (cheveux lisses), Pelo rubio (cheveux blonds), Pelo castaño (cheveux châtains), Pelo negro (cheveux noirs)']) couplet=LyricsSection(lines=['A: ¿Cómo es él? (Comment est-il ?)', 'B: Él es alto y tiene el pelo corto. (Il est grand et a les cheveux courts.)', 'A: ¿De qué color son sus ojos? (De quelle couleur sont ses yeux ?)', 'B: Tiene ojos marrones. (Il a les yeux marron.)', 'A: ¿Qué lleva puesto? (Que porte-t-il ?)', 'B: Lleva una camiseta azul y pantalones negros. (Il porte un t-shirt bleu et un pantalon noir.)']) refrain_2=LyricsSection(lines=['Cheveux (Pelo) :', 'Pelo largo (cheveux longs), Pelo corto (cheveux courts), Pelo rizado (cheveux bouclés), Pelo liso (cheveux lisses), Pelo rubio (cheveux blonds), Pelo castaño (cheveux châtains), Pelo negro (cheveux noirs)']) mini_dialogue=LyricsSection(lines=['A: ¿Es delgado o gordo? (Est-il mince ou gros ?)', 'B: Es delgado. (Il est mince.)']) outro=LyricsSection(lines=["Ahora sabes describir a alguien. ¡Bien hecho! (Maintenant tu sais décrire quelqu'un. Bien joué !)"])</t>
         </is>
       </c>
     </row>
@@ -881,12 +881,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Apprendre les nombres de 11 à 20</t>
+          <t>Décrire une personne (personnalité)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">comment dire 11 à 20 en anglais </t>
+          <t>Apprendre à décrire la personnalité avec des adjectifs simples (ex : simpático/a, divertido/a, tímido/a).</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -896,12 +896,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>{'Introduction': "Hey, let's learn to count, from eleven to twenty, It's easy and fun, you'll see, plenty!", 'Refrain': "Thirteen, fourteen, fifteen, sixteen, (Treize, quatorze, quinze, seize,) Seventeen, eighteen, nineteen, a routine. (Dix-sept, dix-huit, dix-neuf, une routine.) End with twenty, a new decade, (Finis avec vingt, une nouvelle décennie,) Counting in English, you've got it made! (Compter en anglais, tu l'as réussi!)", 'Dialogue': "Personnage A: What's after ten? (Qu'est-ce qui vient après dix?) Personnage B: Eleven, it's unique, my friend. (Onze, c'est unique, mon ami.) Personnage A: And then? (Et ensuite?) Personnage B: Twelve, before we reach the teens. (Douze, avant d'atteindre les ados.) Personnage A: How do we say thirteen? (Comment dit-on treize?) Personnage B: Thirteen, with '-teen', it's keen. (Treize, avec '-teen', c'est astucieux.) Personnage A: What about fourteen? (Et quatorze?) Personnage B: Fourteen, just add '-teen'. (Quatorze, ajoute juste '-teen'.)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprender a describir la personalidad en español con adjetivos simples es una excelente manera de empezar a hablar de uno mismo y de los demás. (Apprendre à décrire la personnalité en espagnol avec des adjectifs simples est une excellente façon de commencer à parler de soi-même et des autres.)']) refrain_1=LyricsSection(lines=['Simpático/a - Sympathique', 'Divertido/a - Amusant(e)', 'Tímido/a - Timide']) couplet=LyricsSection(lines=['A: ¿Cómo es tu amigo? (Comment est ton ami ?)', 'B: Es muy simpático. (Il est très sympathique.)', 'A: ¿Y tu hermana? (Et ta sœur ?)', 'B: Ella es divertida y un poco tímida. (Elle est amusante et un peu timide.)', "A: ¡Qué interesante! (C'est intéressant !)"]) refrain_2=LyricsSection(lines=['Simpático/a - Sympathique', 'Divertido/a - Amusant(e)', 'Tímido/a - Timide']) mini_dialogue=LyricsSection(lines=['A: ¿Eres trabajador? (Es-tu travailleur ?)', 'B: Sí, pero a veces soy perezoso. (Oui, mais parfois je suis paresseux.)']) outro=LyricsSection(lines=["Estos adjetivos te permitirán empezar a describir la personalidad de las personas a tu alrededor en español. ¡No dudes en usarlos en frases para practicar! (Ces adjectifs te permettront de commencer à décrire la personnalité des gens autour de toi en espagnol. N'hésite pas à les utiliser dans des phrases pour t'entraîner !)"])</t>
         </is>
       </c>
     </row>
@@ -921,12 +921,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Utiliser les nombres pour parler de son âge</t>
+          <t>Dire ce qu’on aime et ce qu’on n’aime pas (me gusta / no me gusta)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>apprendre à Utiliser les nombres pour parler de son âge ("J'ai ... ans")</t>
+          <t>Apprendre à exprimer ses goûts et dégoûts avec 'me gusta / no me gusta' (ex : Me gusta bailar).</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -936,12 +936,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, apprendre à dire son âge en anglais, c'est facile, écoute ça !", 'Refrain': "I am [nombre] years old (J'ai [nombre] ans), c'est comme ça qu'on dit son âge.", 'Couplet': "Personnage A: Hey, how old are you? (Hé, quel âge as-tu ?)\nPersonnage B: I am ten years old (J'ai dix ans), et toi ?\nPersonnage A: I am twelve years old (J'ai douze ans), c'est cool !\nPersonnage B: My brother is twenty-one years old (Mon frère a vingt et un ans).\nPersonnage A: Wow, my sister is twenty-five years old (Wow, ma sœur a vingt-cinq ans) !", 'Conclusion': 'Pratique ces phrases, mémorise les nombres, et parle de ton âge facilement.'}</t>
+          <t>introduction=LyricsSection(lines=["Aprender a expresar lo que te gusta y lo que no te gusta es fundamental. (Apprendre à exprimer ce qu'on aime et ce qu'on n'aime pas est fondamental.)"]) refrain_1=LyricsSection(lines=["Me gusta bailar. (J'aime danser.)", "Me gusta el chocolate. (J'aime le chocolat.)"]) couplet=LyricsSection(lines=['A: ¿Te gusta el fútbol? (Aimes-tu le football ?)', "B: Sí, me gusta mucho. (Oui, j'aime beaucoup.)", 'A: ¿Y te gusta la música? (Et aimes-tu la musique ?)', "B: No, no me gusta. (Non, je n'aime pas.)", "A: Me gusta leer libros. (J'aime lire des livres.)", 'B: A mí también. (Moi aussi.)']) refrain_2=LyricsSection(lines=["Me gusta bailar. (J'aime danser.)", "Me gusta el chocolate. (J'aime le chocolat.)"]) mini_dialogue=LyricsSection(lines=['¿Te gusta el café? (Aimes-tu le café ?)', 'Le gusta leer. (Il/elle aime lire.)']) outro=LyricsSection(lines=["Para practicar, intenta hacer frases con 'me gusta' y 'no me gusta'. (Pour pratiquer, essayez de faire des phrases en utilisant 'me gusta' et 'no me gusta'.)"])</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Dire son numéro de téléphone (avec les nombres</t>
+          <t>Parler de ses loisirs / passions</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>apprendre à Dire son numéro de téléphone (avec les nombres)</t>
+          <t>Apprendre à parler de ses loisirs et centres d’intérêt (ex : Me gusta leer, Me encanta el deporte).</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -976,12 +976,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, apprenons à dire notre numéro de téléphone en anglais, c'est pratique et utile !", 'Refrain': 'One two three, four five six, seven eight nine zero. (Un deux trois, quatre cinq six, sept huit neuf zéro.)', 'Couplet 1': "Personnage A: What's your phone number? (Quel est ton numéro de téléphone ?)\nPersonnage B: It's three four five, six seven eight. (C'est trois quatre cinq, six sept huit.)\nPersonnage A: And the area code? (Et le code régional ?)\nPersonnage B: It's zero one two. (C'est zéro un deux.)", 'Couplet 2': "Personnage A: How do you say repeated numbers? (Comment dis-tu les chiffres répétés ?)\nPersonnage B: Use 'double', like double three. (Utilise 'double', comme double trois.)\nPersonnage A: So, double one is? (Donc, double un c'est ?)\nPersonnage B: Eleven! (Onze !)", 'Couplet 3': 'Personnage A: Can you give me an example? (Peux-tu me donner un exemple ?)\nPersonnage B: Sure, nine eight seven, six five four. (Bien sûr, neuf huit sept, six cinq quatre.)\nPersonnage A: And the last part? (Et la dernière partie ?)\nPersonnage B: Three two one zero. (Trois deux un zéro.)', 'Conclusion': 'Écoutez et répétez, améliorez votre prononciation et fluidité !'}</t>
+          <t>introduction=LyricsSection(lines=['Parler de ses loisirs et passions est un excellent moyen de pratiquer une nouvelle langue.', 'Hablar de tus pasatiempos y pasiones es una excelente manera de practicar un nuevo idioma.']) refrain_1=LyricsSection(lines=["Me gusta... (J'aime...)", "Me encanta... (J'adore...)"]) couplet=LyricsSection(lines=["A: ¿Qué te gusta hacer? (Qu'aimes-tu faire ?)", "B: Me gusta leer. (J'aime lire.)", 'A: ¿Te gusta el deporte? (Aimes-tu le sport ?)', "B: Me encanta el deporte. (J'adore le sport.)", 'A: ¿Y la música? (Et la musique ?)', "B: Me gusta escuchar música. (J'aime écouter de la musique.)"]) refrain_2=LyricsSection(lines=["Me gusta... (J'aime...)", "Me encanta... (J'adore...)"]) mini_dialogue=LyricsSection(lines=["¿Qué te gusta hacer en tu tiempo libre? (Qu'aimes-tu faire pendant ton temps libre ?)", '¿Tienes algún pasatiempo? (As-tu un passe-temps ?)']) outro=LyricsSection(lines=["En mi tiempo libre, me gusta... (Dans mon temps libre, j'aime...)", "A menudo, me gusta salir a caminar. (Souvent, j'aime aller me promener.)"])</t>
         </is>
       </c>
     </row>
@@ -1001,12 +1001,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Apprendre les dizaines</t>
+          <t>Dire ce qu’on fait dans la vie (profession, études)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Apprendre les dizaines (20, 30, 40, etc.)</t>
+          <t>Apprendre à dire sa profession ou ses études (ex : Soy estudiante, Trabajo en una oficina).</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1016,12 +1016,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, écoute bien, on va compter, \nLes dizaines en anglais, c'est facile, tu vas voir!", 'Refrain': "Vingt, trente, quarante, cinquante, \nSoixante, soixante-dix, c'est excitant! \nQuatre-vingts, quatre-vingt-dix, cent, \nLes dizaines, c'est important!", 'Couplet': "Personnage A: Hey, do you know twenty (Vingt)? \nPersonnage B: Yes, twenty apples (Vingt pommes) in my bag. \nPersonnage A: And thirty (Trente), can you say it? \nPersonnage B: Thirty books (Trente livres) on the shelf, I see it! \nPersonnage A: What about forty (Quarante)? \nPersonnage B: Forty cars (Quarante voitures) on the street, that's plenty! \nPersonnage A: Fifty (Cinquante), do you know? \nPersonnage B: Fifty stars (Cinquante étoiles) in the sky, they glow!"}</t>
+          <t>introduction=LyricsSection(lines=["Aprender a decir lo que hacemos es esencial. - Apprendre à dire ce que l'on fait est essentiel."]) refrain_1=LyricsSection(lines=['Soy estudiante. - Je suis étudiant(e).', 'Trabajo en una oficina. - Je travaille dans un bureau.', 'Soy profesor/profesora. - Je suis professeur/professeure.']) couplet=LyricsSection(lines=['A: ¿Qué haces tú? - Que fais-tu ?', 'B: Soy médico/médica. - Je suis médecin.', 'A: ¿Y tú? - Et toi ?', 'B: Soy ingeniero/ingeniera. - Je suis ingénieur/ingénieure.', 'A: Trabajo en un hospital. - Je travaille dans un hôpital.', 'B: Soy enfermero/enfermera. - Je suis infirmier/infirmière.']) refrain_2=LyricsSection(lines=['Soy estudiante. - Je suis étudiant(e).', 'Trabajo en una oficina. - Je travaille dans un bureau.', 'Soy profesor/profesora. - Je suis professeur/professeure.']) mini_dialogue=LyricsSection(lines=['A: ¿Dónde estudias? - Où étudies-tu ?', "B: Estudio en la universidad. - J'étudie à l'université.", "A: ¿Qué estudias? - Qu'étudies-tu ?", "B: Estudio ingeniería. - J'étudie l'ingénierie."]) outro=LyricsSection(lines=["Practica estas frases para mejorar. - Pratique ces phrases pour t'améliorer."])</t>
         </is>
       </c>
     </row>
@@ -1041,12 +1041,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Apprendre à compter de 21 à 50</t>
+          <t>Décrire une journée type (emploi du temps simple)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Apprendre à compter de 21 à 50</t>
+          <t>Apprendre à décrire sa journée type (ex : Me levanto a las 7, Voy al colegio a las 8).</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to count from twenty-one to fifty (Apprenons à compter de vingt et un à cinquante).", 'Refrain': "Count with me, let's go, from twenty-one to fifty, nice and slow (Compte avec moi, allons-y, de vingt et un à cinquante, doucement).", 'Dialogue': "Personnage A: How many apples do you have? (Combien de pommes as-tu?)\nPersonnage B: I have twenty-one apples (J'ai vingt et une pommes).\nPersonnage A: And how many oranges? (Et combien d'oranges?)\nPersonnage B: I have thirty oranges (J'ai trente oranges).\nPersonnage A: Can you count to forty? (Peux-tu compter jusqu'à quarante?)\nPersonnage B: Yes, thirty-one, thirty-two, thirty-three, up to forty (Oui, trente et un, trente-deux, trente-trois, jusqu'à quarante).\nPersonnage A: Great! How about forty-five? (Super ! Et quarante-cinq ?)\nPersonnage B: Forty-one, forty-two, forty-three, forty-four, forty-five (Quarante et un, quarante-deux, quarante-trois, quarante-quatre, quarante-cinq)."}</t>
+          <t>introduction=LyricsSection(lines=['Me levanto a las 7 de la mañana.', 'Je me lève à 7 heures du matin.']) refrain_1=LyricsSection(lines=['Voy al colegio a las 8.', "Je vais à l'école à 8 heures."]) couplet=LyricsSection(lines=['A: ¿A qué hora te levantas?', 'A: À quelle heure te lèves-tu ?', 'B: Me levanto a las 7.', 'B: Je me lève à 7 heures.', 'A: ¿Y a qué hora vas al colegio?', "A: Et à quelle heure vas-tu à l'école ?", 'B: Voy al colegio a las 8.', "B: Je vais à l'école à 8 heures.", 'A: ¿Dónde almuerzas?', 'A: Où déjeunes-tu ?', 'B: Almuerzo en la cafetería.', 'B: Je déjeune à la cafétéria.']) refrain_2=LyricsSection(lines=['Voy al colegio a las 8.', "Je vais à l'école à 8 heures."]) mini_dialogue=LyricsSection(lines=['Ceno con mi familia a las 7 de la tarde.', 'Je dîne avec ma famille à 7 heures du soir.']) outro=LyricsSection(lines=['Me acuesto a las 10 de la noche.', 'Je me couche à 10 heures du soir.'])</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1081,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Apprendre à compter de 51 à 100</t>
+          <t>S’exprimer à l’écrit : écrire un petit texte sur soi</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Apprendre à compter de 51 à 100</t>
+          <t>Apprendre à écrire un texte simple sur soi-même (nom, âge, nationalité, goûts).</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1096,12 +1096,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to count, from fifty-one to one hundred, \nApprenons à compter, de cinquante et un à cent, \nIt's easy and fun, let's get started! \nC'est facile et amusant, commençons!", 'Refrain': "Count with me, from fifty-one to one hundred, \nCompte avec moi, de cinquante et un à cent, \nLearn the numbers, say them loud, \nApprends les chiffres, dis-les fort, \nPractice makes perfect, let's count out loud. \nLa pratique rend parfait, comptons à voix haute.", 'Dialogue': "Personnage A: What's your favorite number between fifty-one and sixty? \nQuel est ton chiffre préféré entre cinquante et un et soixante? \nPersonnage B: I like fifty-five (J'aime cinquante-cinq), it's easy to remember. \nC'est facile à retenir.\nPersonnage A: Can you count from sixty-one to seventy? \nPeux-tu compter de soixante et un à soixante-dix? \nPersonnage B: Sure! Sixty-one, sixty-two, sixty-three, sixty-four, sixty-five, sixty-six, sixty-seven, sixty-eight, sixty-nine, seventy. \nBien sûr! Soixante et un, soixante-deux, soixante-trois, soixante-quatre, soixante-cinq, soixante-six, soixante-sept, soixante-huit, soixante-neuf, soixante-dix.\nPersonnage A: Great! Now let's try from seventy-one to eighty. \nSuper! Maintenant essayons de soixante et onze à quatre-vingts. \nPersonnage B: Seventy-one, seventy-two, seventy-three, seventy-four, seventy-five, seventy-six, seventy-seven, seventy-eight, seventy-nine, eighty. \nSoixante et onze, soixante-douze, soixante-treize, soixante-quatorze, soixante-quinze, soixante-seize, soixante-dix-sept, soixante-dix-huit, soixante-dix-neuf, quatre-vingts."}</t>
+          <t>introduction=LyricsSection(lines=['¡Hola! Me llamo [Ton Nom].', "Bonjour ! Je m'appelle [Ton Nom]."]) refrain_1=LyricsSection(lines=['Tengo [ton âge] años.', "J'ai [ton âge] ans."]) couplet=LyricsSection(lines=['A: ¿De dónde eres?', "A: D'où viens-tu ?", 'B: Soy de [ta nationalité]. Vivo en [ta ville ou pays].', "B: Je suis de [ta nationalité]. J'habite à [ta ville ou pays].", 'A: ¿Qué te gusta hacer?', "A: Qu'aimes-tu faire ?", 'B: Me gusta [tes goûts, par exemple: la música, el fútbol, leer libros].', "B: J'aime [tes goûts, par exemple: la musique, le football, lire des livres].", 'A: ¿Y qué no te gusta?', "A: Et qu'est-ce que tu n'aimes pas ?", "B: No me gusta [ce que tu n'aimes pas, par exemple: el pescado, el frío].", "B: Je n'aime pas [ce que tu n'aimes pas, par exemple: le poisson, le froid]."]) refrain_2=LyricsSection(lines=['Tengo [ton âge] años.', "J'ai [ton âge] ans."]) mini_dialogue=LyricsSection(lines=['A: ¿Tienes hermanos?', 'A: As-tu des frères et sœurs ?', 'B: Tengo una familia pequeña/grande.', "B: J'ai une petite/grande famille.", 'B: Tengo [nombre de frères et sœurs, si tu en as].', "B: J'ai [nombre de frères et sœurs, si tu en as]."]) outro=LyricsSection(lines=['Mi color favorito es [ta couleur préférée].', 'Ma couleur préférée est [ta couleur préférée].', 'Mi comida favorita es [ton plat préféré].', 'Mon plat préféré est [ton plat préféré].', 'Estoy aprendiendo español y me gusta mucho.', "J'apprends l'espagnol et j'aime beaucoup."])</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Utiliser les nombres pour parler de prix</t>
+          <t>S’exprimer à l’écrit : écrire un petit texte sur un proche</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>apprendre à Utiliser les nombres pour parler de prix ("Ça coûte ... euros")</t>
+          <t>Apprendre à écrire un texte simple sur une autre personne (ex : Mi hermano se llama..., Tiene... años).</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1136,12 +1136,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn to use numbers to talk about prices. (Apprenons à utiliser les nombres pour parler des prix.)", 'Refrain': 'It costs five euros, it costs ten euros, it costs twenty euros. (Ça coûte cinq euros, ça coûte dix euros, ça coûte vingt euros.)', 'Couplet': 'Person A: How much is this book? (Combien coûte ce livre ?)\nPerson B: It costs fifteen euros. (Ça coûte quinze euros.)\nPerson A: And this pen? (Et ce stylo ?)\nPerson B: It costs two euros. (Ça coûte deux euros.)\nPerson A: What about the notebook? (Et le cahier ?)\nPerson B: It costs three euros and fifty cents. (Ça coûte trois euros et cinquante centimes.)\nPerson A: How much for the backpack? (Combien pour le sac à dos ?)\nPerson B: It costs twenty-five euros. (Ça coûte vingt-cinq euros.)'}</t>
+          <t>introduction=LyricsSection(lines=['Hoy vamos a conocer a Juan.', "(Aujourd'hui, nous allons rencontrer Juan.)"]) refrain_1=LyricsSection(lines=['Juan tiene 15 años, vive en Madrid.', '(Juan a 15 ans, il vit à Madrid.)', 'Le gusta el fútbol y la pizza también.', '(Il aime le football et aussi la pizza.)']) couplet=LyricsSection(lines=['A: ¿Cómo se llama tu hermano?', "(A: Comment s'appelle ton frère ?)", 'B: Mi hermano se llama Juan.', "(B: Mon frère s'appelle Juan.)", 'A: ¿Cuántos años tiene?', '(A: Quel âge a-t-il ?)', 'B: Tiene 15 años.', '(B: Il a 15 ans.)', 'A: ¿Dónde vive?', '(A: Où vit-il ?)', 'B: Vive en Madrid con nuestra familia.', '(B: Il vit à Madrid avec notre famille.)', 'A: ¿Qué le gusta hacer?', "(A: Qu'aime-t-il faire ?)", 'B: Le gusta jugar al fútbol y escuchar música.', '(B: Il aime jouer au football et écouter de la musique.)']) refrain_2=LyricsSection(lines=['Juan tiene 15 años, vive en Madrid.', '(Juan a 15 ans, il vit à Madrid.)', 'Le gusta el fútbol y la pizza también.', '(Il aime le football et aussi la pizza.)']) mini_dialogue=LyricsSection(lines=['A: ¿Es simpático?', '(A: Est-il sympathique ?)', 'B: Sí, siempre me ayuda con mis deberes.', "(B: Oui, il m'aide toujours avec mes devoirs.)"]) outro=LyricsSection(lines=['¡Hasta luego, Juan!', '(À bientôt, Juan !)'])</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Apprendre les couleurs primaires </t>
+          <t>Formuler des phrases au présent simple; La maison : les pièces</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Apprendre les couleurs primaires (rouge, bleu, jaune)</t>
+          <t>Apprendre à utiliser le présent simple pour décrire des actions et parler de la maison.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1176,12 +1176,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>{'Introduction': "Let's learn colors, red, blue, yellow, it's fun! (Apprenons les couleurs, rouge, bleu, jaune, c'est amusant!)", 'Refrain': 'Red, blue, yellow, colors we see. (Rouge, bleu, jaune, couleurs que nous voyons.) Easy as one, two, three! (Facile comme un, deux, trois!)', 'Dialogue': "Personnage A: What color is the apple? (Quelle couleur est la pomme?)\nPersonnage B: It's red, like a fire truck! (Elle est rouge, comme un camion de pompiers!)\nPersonnage A: And the sky, what color is it? (Et le ciel, de quelle couleur est-il?)\nPersonnage B: It's blue, like the ocean! (Il est bleu, comme l'océan!)\nPersonnage A: What about the banana? (Et la banane?)\nPersonnage B: It's yellow, like the sun! (Elle est jaune, comme le soleil!)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprendamos el presente simple en la casa.', '(Apprenons le présent simple dans la maison.)']) refrain_1=LyricsSection(lines=['Yo hablo, tú hablas, él habla.', '(Je parle, tu parles, il parle.)', 'Nosotros vivimos, ellos viven.', '(Nous vivons, ils vivent.)']) couplet=LyricsSection(lines=['A: ¿Qué haces en la cocina?', '(A: Que fais-tu dans la cuisine?)', 'B: Yo cocino y tú comes.', '(B: Je cuisine et tu manges.)', 'A: ¿Dónde está el salón?', '(A: Où est le salon?)', 'B: Está al lado del comedor.', '(B: Il est à côté de la salle à manger.)', 'A: ¿Qué haces en el dormitorio?', '(A: Que fais-tu dans la chambre?)', 'B: Yo duermo y descanso.', '(B: Je dors et je me repose.)']) refrain_2=LyricsSection(lines=['Yo hablo, tú hablas, él habla.', '(Je parle, tu parles, il parle.)', 'Nosotros vivimos, ellos viven.', '(Nous vivons, ils vivent.)']) mini_dialogue=LyricsSection(lines=['A: ¿Dónde vives?', '(A: Où habites-tu?)', 'B: Vivo en una casa con jardín.', "(B: J'habite dans une maison avec jardin.)"]) outro=LyricsSection(lines=['Practiquemos el presente simple cada día.', '(Pratiquons le présent simple chaque jour.)'])</t>
         </is>
       </c>
     </row>
@@ -1201,12 +1201,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Associer les couleurs à des objets</t>
+          <t>La maison : les meubles</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Associer les couleurs à des objets ("La pomme est rouge")</t>
+          <t>Apprendre à nommer les meubles dans une maison et à les décrire simplement.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, let's learn colors, it's easy and fun (Yo, apprenons les couleurs, c'est facile et amusant)", 'Refrain': 'Colors everywhere, in all that we see (Les couleurs partout, dans tout ce que nous voyons)\nRed, blue, yellow, green, learn them with me (Rouge, bleu, jaune, vert, apprends-les avec moi)', 'Dialogue': "Personnage A: What's the color of the apple? (Quelle est la couleur de la pomme?)\nPersonnage B: The apple is red, can't you see? (La pomme est rouge, tu ne vois pas?)\nPersonnage A: And the sky above us? (Et le ciel au-dessus de nous?)\nPersonnage B: The sky is blue, so high and free. (Le ciel est bleu, si haut et libre)\nPersonnage A: What about the banana? (Et la banane?)\nPersonnage B: The banana is yellow, bright as can be. (La banane est jaune, aussi brillante que possible)\nPersonnage A: And the grass under our feet? (Et l'herbe sous nos pieds?)\nPersonnage B: The grass is green, like a leafy sea. (L'herbe est verte, comme une mer feuillue)"}</t>
+          <t>introduction=LyricsSection(lines=['Aprendamos a nombrar los muebles en español. (Apprenons à nommer les meubles en espagnol.)']) refrain_1=LyricsSection(lines=["La cama (le lit) : Es un mueble donde dormimos. Tiene un colchón y a veces almohadas y mantas. (C'est un meuble où nous dormons. Il a un matelas et parfois des oreillers et des couvertures.)", "La mesa (la table) : Es un mueble con una superficie plana. Usamos la mesa para comer o trabajar. (C'est un meuble avec une surface plane. Nous utilisons la table pour manger ou travailler.)", "La silla (la chaise) : Es un mueble para sentarse. Tiene un respaldo y a veces brazos. (C'est un meuble pour s'asseoir. Il a un dossier et parfois des accoudoirs.)"]) couplet=LyricsSection(lines=["A: ¿Qué hay en tu sala? (Qu'y a-t-il dans ton salon ?)", 'B: Hay un sofá grande y cómodo. (Il y a un grand canapé confortable.)', 'A: ¿Tienes un armario en tu habitación? (As-tu une armoire dans ta chambre ?)', "B: Sí, tengo un armario para mi ropa. (Oui, j'ai une armoire pour mes vêtements.)", 'A: ¿Dónde pones tus libros? (Où mets-tu tes livres ?)', "B: Los pongo en la estantería. (Je les mets sur l'étagère.)"]) refrain_2=LyricsSection(lines=["La cama (le lit) : Es un mueble donde dormimos. Tiene un colchón y a veces almohadas y mantas. (C'est un meuble où nous dormons. Il a un matelas et parfois des oreillers et des couvertures.)", "La mesa (la table) : Es un mueble con una superficie plana. Usamos la mesa para comer o trabajar. (C'est un meuble avec une surface plane. Nous utilisons la table pour manger ou travailler.)", "La silla (la chaise) : Es un mueble para sentarse. Tiene un respaldo y a veces brazos. (C'est un meuble pour s'asseoir. Il a un dossier et parfois des accoudoirs.)"]) mini_dialogue=LyricsSection(lines=['En mi sala, hay un sofá grande y una mesa pequeña. (Dans mon salon, il y a un grand canapé et une petite table.)']) outro=LyricsSection(lines=['Esto te ayudará a familiarizarte con el vocabulario y mejorar tu capacidad para describir objetos en español. (Cela vous aidera à vous familiariser avec le vocabulaire et à améliorer votre capacité à décrire des objets en espagnol.)'])</t>
         </is>
       </c>
     </row>
@@ -1241,12 +1241,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Utiliser des couleurs pour décrire des vêtements</t>
+          <t>Les objets du quotidien</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>apprendre à Utiliser des couleurs pour décrire des vêtements ("Il/Elle porte un pull bleu")</t>
+          <t>Apprendre à identifier et nommer les objets du quotidien (ex : el bolígrafo, la mochila...).</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1256,12 +1256,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, écoute bien, on va apprendre,\nLes couleurs et les vêtements, c'est le plan.", 'Refrain': "Il/Elle porte, c'est facile à dire,\nUn vêtement coloré, à décrire.\nPratique chaque jour, avec passion,\nLes couleurs et les vêtements, en toute saison.", 'Couplet': 'Personnage A: What color is your shirt? (De quelle couleur est ta chemise?)\nPersonnage B: My shirt is red. (Ma chemise est rouge.)\nPersonnage A: And your pants? (Et ton pantalon?)\nPersonnage B: They are black. (Ils sont noirs.)\nPersonnage A: What about your shoes? (Et tes chaussures?)\nPersonnage B: My shoes are white. (Mes chaussures sont blanches.)\nPersonnage A: Is your hat blue? (Ton chapeau est-il bleu?)\nPersonnage B: Yes, it is blue. (Oui, il est bleu.)'}</t>
+          <t>introduction=LyricsSection(lines=['Vamos a aprender los nombres de los objetos del día a día. (Nous allons apprendre les noms des objets du quotidien.)']) refrain_1=LyricsSection(lines=['El bolígrafo - Le stylo', 'La mochila - Le sac à dos', 'El libro - Le livre', 'La mesa - La table', 'La silla - La chaise']) couplet=LyricsSection(lines=["A: ¿Qué es esto? (Qu'est-ce que c'est ?)", "B: Es un cuaderno. (C'est un cahier.)", 'A: ¿Y eso? (Et ça ?)', "B: Es un lápiz. (C'est un crayon.)", 'A: ¿Dónde está la ventana? (Où est la fenêtre ?)', 'B: Está al lado de la puerta. (Elle est à côté de la porte.)', 'A: ¿Tienes un teléfono? (As-tu un téléphone ?)', 'B: Sí, aquí está. (Oui, le voici.)']) refrain_2=LyricsSection(lines=['El bolígrafo - Le stylo', 'La mochila - Le sac à dos', 'El libro - Le livre', 'La mesa - La table', 'La silla - La chaise']) mini_dialogue=LyricsSection(lines=["A: ¿Qué es eso en la mesa? (Qu'est-ce que c'est sur la table ?)", "B: Es un plato. (C'est une assiette.)"]) outro=LyricsSection(lines=['Practica nombrando objetos en español. (Pratiquez en nommant les objets en espagnol.)', '¡Buena suerte! (Bonne chance !)'])</t>
         </is>
       </c>
     </row>
@@ -1281,13 +1281,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Apprendre les jours de la semaine</t>
+          <t>Les vêtements</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Apprendre les jours de la semaine (lundi, mardi, etc.
-</t>
+          <t>Apprendre à nommer les vêtements et les associer à des situations simples (ex : Llevo una camiseta).</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1297,12 +1296,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>anglais</t>
+          <t>espagnol</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1312,7 +1311,47 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>{'Introduction': "Yo, écoute bien, on va apprendre les jours, en anglais et en français, c'est parti !", 'Refrain': 'Monday, Tuesday, Wednesday, Thursday, Friday, Saturday, Sunday. (Lundi, mardi, mercredi, jeudi, vendredi, samedi, dimanche.)', 'Couplet': "Personnage A: What's today? (Quel jour sommes-nous ?) Personnage B: Today is Monday. (Aujourd'hui c'est lundi.) Personnage A: And tomorrow? (Et demain ?) Personnage B: Tomorrow is Tuesday. (Demain c'est mardi.) Personnage A: What about yesterday? (Et hier ?) Personnage B: Yesterday was Sunday. (Hier c'était dimanche.) Personnage A: What's your favorite day? (Quel est ton jour préféré ?) Personnage B: I love Saturday! (J'adore le samedi !)"}</t>
+          <t>introduction=LyricsSection(lines=['Es importante aprender a nombrar la ropa en español.', "Il est important d'apprendre à nommer les vêtements en espagnol."]) refrain_1=LyricsSection(lines=['Llevo una camiseta en casa.', 'Je porte un t-shirt à la maison.']) couplet=LyricsSection(lines=['A: ¿Qué llevas al trabajo?', 'A: Que portes-tu au travail?', 'B: Llevo pantalones y una camisa.', 'B: Je porte un pantalon et une chemise.', 'A: ¿Y en la playa?', 'A: Et à la plage?', 'B: Llevo un sombrero y sandalias.', 'B: Je porte un chapeau et des sandales.', 'A: ¿Qué llevas cuando hace frío?', 'A: Que portes-tu quand il fait froid?', 'B: Llevo una chaqueta y un abrigo.', 'B: Je porte une veste et un manteau.']) refrain_2=LyricsSection(lines=['Llevo una camiseta en casa.', 'Je porte un t-shirt à la maison.']) mini_dialogue=LyricsSection(lines=['¿Qué llevas hoy?', 'Hoy llevo una camiseta y pantalones.', "Que portes-tu aujourd'hui?", "Aujourd'hui, je porte un t-shirt et un pantalon."]) outro=LyricsSection(lines=['Practica estas frases para mejorar tu vocabulario.', 'Pratiquez ces phrases pour améliorer votre vocabulaire.'])</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Les couleurs</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Apprendre à nommer et utiliser les couleurs pour décrire des objets ou des vêtements.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>RAP CLASSIQUE</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>espagnol</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>espagnol</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>introduction=LyricsSection(lines=['Aprendamos los colores en español para describir objetos y ropa.', '(Apprenons les couleurs en espagnol pour décrire des objets et des vêtements.)']) refrain_1=LyricsSection(lines=['Rojo, la manzana es roja.', '(Rouge, la pomme est rouge.)', 'Azul, el cielo es azul.', '(Bleu, le ciel est bleu.)', 'Verde, la hoja es verde.', '(Vert, la feuille est verte.)']) couplet=LyricsSection(lines=['A: ¿De qué color es el sol? (De quelle couleur est le soleil?)', 'B: El sol es amarillo. (Le soleil est jaune.)', 'A: ¿Y el gato? (Et le chat?)', 'B: El gato es negro. (Le chat est noir.)', 'A: ¿La nieve? (La neige?)', 'B: La nieve es blanca. (La neige est blanche.)']) refrain_2=LyricsSection(lines=['Rojo, la manzana es roja.', '(Rouge, la pomme est rouge.)', 'Azul, el cielo es azul.', '(Bleu, le ciel est bleu.)', 'Verde, la hoja es verde.', '(Vert, la feuille est verte.)']) mini_dialogue=LyricsSection(lines=['A: La camiseta es azul. (Le t-shirt est bleu.)', 'B: Los pantalones son negros. (Le pantalon est noir.)', 'A: El vestido es rojo. (La robe est rouge.)']) outro=LyricsSection(lines=['¡Practica describiendo los colores de los objetos a tu alrededor en español!', '(Pratique en essayant de décrire les couleurs des objets autour de toi en espagnol !)'])</t>
         </is>
       </c>
     </row>

</xml_diff>